<commit_message>
AE-100 implement pages 5-8 of energiatodistus pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$1:$G$78</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$J$55</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm.Print_Area" vbProcedure="false">'6) huomiot 1'!$B$2:$F$53</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">'7) huomiot 2'!$B$2:$F$61</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$H$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'1) etusivu'!$A$1:$Q$50</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'2) E-luokka'!$B$2:$K$59</definedName>
@@ -32,7 +32,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'4) E-luvun laskennan tulokset '!$B$2:$G$76</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'5) toteutunut kulutus'!$B$2:$K$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'6) huomiot 1'!$B$2:$G$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'7) huomiot 2'!$B$2:$G$59</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="Z_202E1614_C6AB_4311_B593_89481D56C4C7_.wvu.PrintArea" vbProcedure="false">'8) lisämerkintöjä'!$B$2:$I$62</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="211">
   <si>
     <t xml:space="preserve">ENERGIATODISTUS 2018</t>
   </si>
@@ -1602,7 +1602,7 @@
     <numFmt numFmtId="169" formatCode="@"/>
     <numFmt numFmtId="170" formatCode="0"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1882,6 +1882,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF339966"/>
@@ -1956,7 +1963,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC40009"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
   </fills>
@@ -2367,7 +2374,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -3318,11 +3325,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="170" fontId="38" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="170" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3378,10 +3389,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -3390,6 +3397,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -3442,11 +3453,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3571,7 +3578,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="379">
+  <dxfs count="363">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -5287,118 +5294,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
@@ -6311,7 +6206,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
@@ -6342,7 +6237,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFFF4000"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -6362,9 +6257,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
+      <xdr:colOff>249120</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6378,7 +6273,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="759600" cy="216360"/>
+          <a:ext cx="759240" cy="216000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6399,9 +6294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>149400</xdr:colOff>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6415,7 +6310,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1103040" cy="216360"/>
+          <a:ext cx="1102680" cy="216000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6436,9 +6331,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>22680</xdr:colOff>
+      <xdr:colOff>22320</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6452,7 +6347,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1409760" cy="216360"/>
+          <a:ext cx="1409400" cy="216000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6473,9 +6368,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>346680</xdr:colOff>
+      <xdr:colOff>346320</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6489,7 +6384,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1733760" cy="216360"/>
+          <a:ext cx="1733400" cy="216000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6510,9 +6405,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>219960</xdr:colOff>
+      <xdr:colOff>219600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>276840</xdr:rowOff>
+      <xdr:rowOff>276480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6526,7 +6421,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2040840" cy="229320"/>
+          <a:ext cx="2040480" cy="228960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6547,9 +6442,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>163080</xdr:colOff>
+      <xdr:colOff>162720</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>263880</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6563,7 +6458,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2377080" cy="216360"/>
+          <a:ext cx="2376720" cy="216000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6584,9 +6479,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>103320</xdr:colOff>
+      <xdr:colOff>102960</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>263520</xdr:rowOff>
+      <xdr:rowOff>263160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6596,7 +6491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530040"/>
-          <a:ext cx="2689920" cy="215280"/>
+          <a:ext cx="2689560" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6965,9 +6860,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>302760</xdr:colOff>
+      <xdr:colOff>302400</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6977,7 +6872,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6989040" cy="10558800"/>
+          <a:ext cx="6988680" cy="10558440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7105,9 +7000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>427320</xdr:colOff>
+      <xdr:colOff>426960</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>297360</xdr:rowOff>
+      <xdr:rowOff>297000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7121,7 +7016,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5087160" y="5274720"/>
-          <a:ext cx="1127520" cy="260640"/>
+          <a:ext cx="1127160" cy="260280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7147,9 +7042,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>149760</xdr:colOff>
+      <xdr:colOff>149400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7159,7 +7054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="201240" y="10549800"/>
-          <a:ext cx="7024320" cy="258840"/>
+          <a:ext cx="7023960" cy="258480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7218,9 +7113,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1014480</xdr:colOff>
+      <xdr:colOff>1014120</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7230,7 +7125,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="396000" y="10928520"/>
-          <a:ext cx="7091640" cy="265680"/>
+          <a:ext cx="7091280" cy="265320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7289,9 +7184,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1018080</xdr:colOff>
+      <xdr:colOff>1017720</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7301,7 +7196,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="290520" y="11094480"/>
-          <a:ext cx="7051320" cy="260280"/>
+          <a:ext cx="7050960" cy="259920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7360,9 +7255,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>34560</xdr:colOff>
+      <xdr:colOff>34200</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7372,7 +7267,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="241920" y="9930960"/>
-          <a:ext cx="6890400" cy="259560"/>
+          <a:ext cx="6890040" cy="259200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7431,9 +7326,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>52920</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7443,7 +7338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="170640" y="10200240"/>
-          <a:ext cx="6986880" cy="360360"/>
+          <a:ext cx="6986520" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7497,13 +7392,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>360</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>62640</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:colOff>62280</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
@@ -7513,8 +7408,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="163440" y="10173240"/>
-          <a:ext cx="6995880" cy="371520"/>
+          <a:off x="163440" y="10335960"/>
+          <a:ext cx="6995520" cy="371160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7573,9 +7468,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7585,7 +7480,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="90720" y="9993600"/>
-          <a:ext cx="7036200" cy="371520"/>
+          <a:ext cx="7035840" cy="371160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7640,7 +7535,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ51"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="U32" activeCellId="0" sqref="U32"/>
     </sheetView>
   </sheetViews>
@@ -12541,8 +12436,8 @@
   </sheetPr>
   <dimension ref="B2:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F70" activeCellId="0" sqref="F70"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F68" activeCellId="0" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13912,7 +13807,7 @@
   <dimension ref="B2:AMJ55"/>
   <sheetViews>
     <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14157,7 +14052,9 @@
       <c r="F12" s="76"/>
       <c r="G12" s="281"/>
       <c r="H12" s="180"/>
-      <c r="I12" s="282"/>
+      <c r="I12" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J12" s="283"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14168,7 +14065,7 @@
       <c r="F13" s="76"/>
       <c r="G13" s="281"/>
       <c r="H13" s="180"/>
-      <c r="I13" s="282"/>
+      <c r="I13" s="284"/>
       <c r="J13" s="283"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14181,7 +14078,9 @@
       <c r="F14" s="76"/>
       <c r="G14" s="281"/>
       <c r="H14" s="180"/>
-      <c r="I14" s="282"/>
+      <c r="I14" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J14" s="283"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14192,12 +14091,12 @@
       <c r="F15" s="76"/>
       <c r="G15" s="281"/>
       <c r="H15" s="180"/>
-      <c r="I15" s="282"/>
+      <c r="I15" s="284"/>
       <c r="J15" s="283"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="98"/>
-      <c r="C16" s="284" t="s">
+      <c r="C16" s="285" t="s">
         <v>173</v>
       </c>
       <c r="D16" s="101"/>
@@ -14205,12 +14104,14 @@
       <c r="F16" s="76"/>
       <c r="G16" s="281"/>
       <c r="H16" s="180"/>
-      <c r="I16" s="282"/>
+      <c r="I16" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J16" s="283"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="98"/>
-      <c r="C17" s="284" t="s">
+      <c r="C17" s="285" t="s">
         <v>174</v>
       </c>
       <c r="D17" s="101"/>
@@ -14218,18 +14119,20 @@
       <c r="F17" s="76"/>
       <c r="G17" s="281"/>
       <c r="H17" s="180"/>
-      <c r="I17" s="282"/>
+      <c r="I17" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J17" s="283"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="98"/>
-      <c r="C18" s="284"/>
+      <c r="C18" s="285"/>
       <c r="D18" s="101"/>
       <c r="E18" s="280"/>
       <c r="F18" s="76"/>
       <c r="G18" s="280"/>
       <c r="H18" s="180"/>
-      <c r="I18" s="282"/>
+      <c r="I18" s="284"/>
       <c r="J18" s="283"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14242,19 +14145,21 @@
       <c r="F19" s="101"/>
       <c r="G19" s="101"/>
       <c r="H19" s="180"/>
-      <c r="I19" s="282"/>
+      <c r="I19" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J19" s="283"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="107"/>
-      <c r="C20" s="285"/>
-      <c r="D20" s="285"/>
-      <c r="E20" s="285"/>
-      <c r="F20" s="285"/>
-      <c r="G20" s="285"/>
+      <c r="C20" s="286"/>
+      <c r="D20" s="286"/>
+      <c r="E20" s="286"/>
+      <c r="F20" s="286"/>
+      <c r="G20" s="286"/>
       <c r="H20" s="202"/>
-      <c r="I20" s="286"/>
-      <c r="J20" s="287"/>
+      <c r="I20" s="287"/>
+      <c r="J20" s="288"/>
     </row>
     <row r="21" s="264" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="272"/>
@@ -14262,22 +14167,22 @@
         <v>175</v>
       </c>
       <c r="D21" s="273"/>
-      <c r="E21" s="288" t="s">
+      <c r="E21" s="289" t="s">
         <v>176</v>
       </c>
-      <c r="F21" s="289" t="s">
+      <c r="F21" s="290" t="s">
         <v>177</v>
       </c>
-      <c r="G21" s="288" t="s">
+      <c r="G21" s="289" t="s">
         <v>178</v>
       </c>
-      <c r="H21" s="289" t="s">
+      <c r="H21" s="290" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="289" t="s">
+      <c r="I21" s="290" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="289"/>
+      <c r="J21" s="290"/>
       <c r="AKP21" s="0"/>
       <c r="AKQ21" s="0"/>
       <c r="AKR21" s="0"/>
@@ -14328,14 +14233,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="92"/>
-      <c r="C22" s="290"/>
-      <c r="D22" s="290"/>
-      <c r="E22" s="291"/>
-      <c r="F22" s="292"/>
-      <c r="G22" s="293"/>
-      <c r="H22" s="293"/>
-      <c r="I22" s="294"/>
-      <c r="J22" s="295"/>
+      <c r="C22" s="291"/>
+      <c r="D22" s="291"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="293"/>
+      <c r="G22" s="294"/>
+      <c r="H22" s="294"/>
+      <c r="I22" s="295"/>
+      <c r="J22" s="296"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="98"/>
@@ -14344,14 +14249,18 @@
       </c>
       <c r="D23" s="101"/>
       <c r="E23" s="180"/>
-      <c r="F23" s="296" t="s">
+      <c r="F23" s="297" t="s">
         <v>180</v>
       </c>
       <c r="G23" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="H23" s="297"/>
-      <c r="I23" s="282"/>
+      <c r="H23" s="282" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J23" s="283"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14361,14 +14270,18 @@
       </c>
       <c r="D24" s="101"/>
       <c r="E24" s="180"/>
-      <c r="F24" s="296" t="s">
+      <c r="F24" s="297" t="s">
         <v>182</v>
       </c>
       <c r="G24" s="121" t="n">
         <v>1300</v>
       </c>
-      <c r="H24" s="297"/>
-      <c r="I24" s="282"/>
+      <c r="H24" s="282" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J24" s="283"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14378,14 +14291,18 @@
       </c>
       <c r="D25" s="101"/>
       <c r="E25" s="180"/>
-      <c r="F25" s="296" t="s">
+      <c r="F25" s="297" t="s">
         <v>182</v>
       </c>
       <c r="G25" s="121" t="n">
         <v>1700</v>
       </c>
-      <c r="H25" s="297"/>
-      <c r="I25" s="282"/>
+      <c r="H25" s="282" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J25" s="283"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14395,14 +14312,18 @@
       </c>
       <c r="D26" s="101"/>
       <c r="E26" s="180"/>
-      <c r="F26" s="296" t="s">
+      <c r="F26" s="297" t="s">
         <v>185</v>
       </c>
       <c r="G26" s="121" t="n">
         <v>4.7</v>
       </c>
-      <c r="H26" s="297"/>
-      <c r="I26" s="282"/>
+      <c r="H26" s="282" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J26" s="283"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14412,8 +14333,8 @@
       <c r="E27" s="180"/>
       <c r="F27" s="299"/>
       <c r="G27" s="180"/>
-      <c r="H27" s="297"/>
-      <c r="I27" s="282"/>
+      <c r="H27" s="300"/>
+      <c r="I27" s="284"/>
       <c r="J27" s="283"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14423,54 +14344,54 @@
       <c r="E28" s="180"/>
       <c r="F28" s="299"/>
       <c r="G28" s="180"/>
-      <c r="H28" s="297"/>
-      <c r="I28" s="282"/>
+      <c r="H28" s="300"/>
+      <c r="I28" s="284"/>
       <c r="J28" s="283"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="98"/>
-      <c r="C29" s="300" t="s">
+      <c r="C29" s="301" t="s">
         <v>186</v>
       </c>
-      <c r="D29" s="300"/>
+      <c r="D29" s="301"/>
       <c r="E29" s="180"/>
       <c r="F29" s="299"/>
       <c r="G29" s="180"/>
-      <c r="H29" s="297"/>
-      <c r="I29" s="282"/>
+      <c r="H29" s="300"/>
+      <c r="I29" s="284"/>
       <c r="J29" s="283"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="98"/>
-      <c r="C30" s="300"/>
-      <c r="D30" s="300"/>
+      <c r="C30" s="301"/>
+      <c r="D30" s="301"/>
       <c r="E30" s="180"/>
       <c r="F30" s="299"/>
       <c r="G30" s="180"/>
-      <c r="H30" s="297"/>
-      <c r="I30" s="282"/>
+      <c r="H30" s="300"/>
+      <c r="I30" s="284"/>
       <c r="J30" s="283"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="98"/>
-      <c r="C31" s="300"/>
-      <c r="D31" s="300"/>
+      <c r="C31" s="301"/>
+      <c r="D31" s="301"/>
       <c r="E31" s="180"/>
       <c r="F31" s="299"/>
       <c r="G31" s="180"/>
-      <c r="H31" s="297"/>
-      <c r="I31" s="282"/>
+      <c r="H31" s="300"/>
+      <c r="I31" s="284"/>
       <c r="J31" s="283"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="98"/>
-      <c r="C32" s="300"/>
-      <c r="D32" s="300"/>
+      <c r="C32" s="301"/>
+      <c r="D32" s="301"/>
       <c r="E32" s="180"/>
       <c r="F32" s="299"/>
       <c r="G32" s="180"/>
-      <c r="H32" s="297"/>
-      <c r="I32" s="282"/>
+      <c r="H32" s="300"/>
+      <c r="I32" s="284"/>
       <c r="J32" s="283"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14480,20 +14401,20 @@
       <c r="E33" s="180"/>
       <c r="F33" s="299"/>
       <c r="G33" s="180"/>
-      <c r="H33" s="297"/>
-      <c r="I33" s="282"/>
+      <c r="H33" s="300"/>
+      <c r="I33" s="284"/>
       <c r="J33" s="283"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="107"/>
-      <c r="C34" s="301"/>
-      <c r="D34" s="301"/>
+      <c r="C34" s="302"/>
+      <c r="D34" s="302"/>
       <c r="E34" s="202"/>
-      <c r="F34" s="302"/>
+      <c r="F34" s="303"/>
       <c r="G34" s="202"/>
-      <c r="H34" s="303"/>
-      <c r="I34" s="286"/>
-      <c r="J34" s="287"/>
+      <c r="H34" s="304"/>
+      <c r="I34" s="287"/>
+      <c r="J34" s="288"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="98"/>
@@ -14504,8 +14425,8 @@
       <c r="E35" s="280"/>
       <c r="F35" s="76"/>
       <c r="G35" s="280"/>
-      <c r="H35" s="304"/>
-      <c r="I35" s="305"/>
+      <c r="H35" s="305"/>
+      <c r="I35" s="306"/>
       <c r="J35" s="283"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14525,14 +14446,14 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="92"/>
-      <c r="C37" s="306"/>
-      <c r="D37" s="306"/>
-      <c r="E37" s="307"/>
-      <c r="F37" s="308"/>
-      <c r="G37" s="308"/>
+      <c r="C37" s="307"/>
+      <c r="D37" s="307"/>
+      <c r="E37" s="308"/>
+      <c r="F37" s="309"/>
+      <c r="G37" s="309"/>
       <c r="H37" s="206"/>
-      <c r="I37" s="309"/>
-      <c r="J37" s="310"/>
+      <c r="I37" s="310"/>
+      <c r="J37" s="311"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="98"/>
@@ -14540,22 +14461,24 @@
         <v>188</v>
       </c>
       <c r="D38" s="30"/>
-      <c r="E38" s="311"/>
-      <c r="F38" s="312"/>
-      <c r="G38" s="312"/>
+      <c r="E38" s="312"/>
+      <c r="F38" s="313"/>
+      <c r="G38" s="313"/>
       <c r="H38" s="180"/>
-      <c r="I38" s="305"/>
+      <c r="I38" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J38" s="283"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="98"/>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
-      <c r="E39" s="311"/>
-      <c r="F39" s="312"/>
-      <c r="G39" s="312"/>
+      <c r="E39" s="312"/>
+      <c r="F39" s="313"/>
+      <c r="G39" s="313"/>
       <c r="H39" s="180"/>
-      <c r="I39" s="305"/>
+      <c r="I39" s="306"/>
       <c r="J39" s="283"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14564,22 +14487,24 @@
         <v>189</v>
       </c>
       <c r="D40" s="30"/>
-      <c r="E40" s="311"/>
-      <c r="F40" s="312"/>
-      <c r="G40" s="312"/>
+      <c r="E40" s="312"/>
+      <c r="F40" s="313"/>
+      <c r="G40" s="313"/>
       <c r="H40" s="180"/>
-      <c r="I40" s="305"/>
+      <c r="I40" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J40" s="283"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="98"/>
       <c r="C41" s="30"/>
       <c r="D41" s="30"/>
-      <c r="E41" s="311"/>
-      <c r="F41" s="312"/>
-      <c r="G41" s="312"/>
+      <c r="E41" s="312"/>
+      <c r="F41" s="313"/>
+      <c r="G41" s="313"/>
       <c r="H41" s="180"/>
-      <c r="I41" s="305"/>
+      <c r="I41" s="306"/>
       <c r="J41" s="283"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14588,22 +14513,24 @@
         <v>190</v>
       </c>
       <c r="D42" s="30"/>
-      <c r="E42" s="311"/>
-      <c r="F42" s="312"/>
-      <c r="G42" s="312"/>
+      <c r="E42" s="312"/>
+      <c r="F42" s="313"/>
+      <c r="G42" s="313"/>
       <c r="H42" s="180"/>
-      <c r="I42" s="305"/>
+      <c r="I42" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J42" s="283"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="98"/>
       <c r="C43" s="30"/>
       <c r="D43" s="30"/>
-      <c r="E43" s="311"/>
-      <c r="F43" s="312"/>
-      <c r="G43" s="312"/>
+      <c r="E43" s="312"/>
+      <c r="F43" s="313"/>
+      <c r="G43" s="313"/>
       <c r="H43" s="180"/>
-      <c r="I43" s="305"/>
+      <c r="I43" s="306"/>
       <c r="J43" s="283"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14612,22 +14539,24 @@
         <v>150</v>
       </c>
       <c r="D44" s="30"/>
-      <c r="E44" s="311"/>
-      <c r="F44" s="312"/>
-      <c r="G44" s="312"/>
+      <c r="E44" s="312"/>
+      <c r="F44" s="313"/>
+      <c r="G44" s="313"/>
       <c r="H44" s="180"/>
-      <c r="I44" s="305"/>
+      <c r="I44" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J44" s="283"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="98"/>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
-      <c r="E45" s="311"/>
-      <c r="F45" s="312"/>
-      <c r="G45" s="312"/>
+      <c r="E45" s="312"/>
+      <c r="F45" s="313"/>
+      <c r="G45" s="313"/>
       <c r="H45" s="180"/>
-      <c r="I45" s="305"/>
+      <c r="I45" s="306"/>
       <c r="J45" s="283"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14639,8 +14568,12 @@
       <c r="E46" s="4"/>
       <c r="F46" s="46"/>
       <c r="G46" s="46"/>
-      <c r="H46" s="122"/>
-      <c r="I46" s="313"/>
+      <c r="H46" s="282" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="282" t="s">
+        <v>14</v>
+      </c>
       <c r="J46" s="314"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14739,7 +14672,7 @@
     <mergeCell ref="I36:J36"/>
     <mergeCell ref="C48:J53"/>
   </mergeCells>
-  <conditionalFormatting sqref="L46:GZ47 L53:GZ54 K53 L37:GZ45 K32:K47 J5:J9 C10 H10 B55:GZ65353 B2:J2 B54:J54 B5:I6 B9:I9 E11:H11 B46:E47 F12:F13 L2:GZ6 B37:D45 B8:D8 F8:I8 K2:K24 L7:GZ7 B4:J4 B3:C3 C35 I19:I20 H12:H20 L8:GZ24 B10:B24 H23:I35 L32:GZ36 B32:B36 E23:E36 G27:G36">
+  <conditionalFormatting sqref="L46:GZ47 L53:GZ54 K53 L37:GZ45 K32:K47 J5:J9 C10 H10 B55:GZ65353 B2:J2 B54:J54 B5:I6 B9:I9 E11:H11 B46:E47 F12:F13 L2:GZ6 B37:D45 B8:D8 F8:I8 K2:K24 L7:GZ7 B4:J4 B3:C3 C35 I20 H12:H20 L8:GZ24 B10:B24 H27:I35 L32:GZ36 B32:B36 E23:E36 G27:G36">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="229">
       <formula>"*"</formula>
     </cfRule>
@@ -15054,213 +14987,133 @@
       <formula>LEFT(F28,1)="*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I13">
+  <conditionalFormatting sqref="I12:I14 I16:I17 I19 H23:I26 I38 I40 I42 I44 H46:I46">
     <cfRule type="cellIs" priority="65" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="292">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:I13">
+  <conditionalFormatting sqref="I12:I14 I16:I17 I19 H23:I26 I38 I40 I42 I44 H46:I46">
     <cfRule type="cellIs" priority="66" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="293">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
+  <conditionalFormatting sqref="I18 I15">
     <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="294">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I46">
+  <conditionalFormatting sqref="I18 I15">
     <cfRule type="cellIs" priority="68" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="295">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I18">
+  <conditionalFormatting sqref="I39 I45 I37 I43">
     <cfRule type="cellIs" priority="69" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="296">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I18">
+  <conditionalFormatting sqref="I39 I45 I37 I43">
     <cfRule type="cellIs" priority="70" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="297">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="F12:F18">
     <cfRule type="cellIs" priority="71" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="298">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25:H26">
+  <conditionalFormatting sqref="F12:F18">
     <cfRule type="cellIs" priority="72" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="299">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:H26">
+  <conditionalFormatting sqref="F12:F18">
     <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="300">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:H26">
+  <conditionalFormatting sqref="F12:F18">
     <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="301">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="E37:E41">
     <cfRule type="cellIs" priority="75" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="302">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
+  <conditionalFormatting sqref="E12:E13">
     <cfRule type="cellIs" priority="76" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="303">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
+  <conditionalFormatting sqref="E14:E18">
     <cfRule type="cellIs" priority="77" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="304">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:H26">
+  <conditionalFormatting sqref="G12:G18">
     <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="305">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H37:H39 H42:H45">
     <cfRule type="cellIs" priority="79" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="306">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:H26">
+  <conditionalFormatting sqref="C21:D22">
     <cfRule type="cellIs" priority="80" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="307">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="E21:E22">
     <cfRule type="cellIs" priority="81" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="308">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
+  <conditionalFormatting sqref="G21:G22">
     <cfRule type="cellIs" priority="82" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="309">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
+  <conditionalFormatting sqref="H21:H22">
     <cfRule type="cellIs" priority="83" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="310">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:I39 I42:I45">
+  <conditionalFormatting sqref="I21:I22">
     <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="311">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:I39 I42:I45">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="312">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F18">
+  <conditionalFormatting sqref="I36">
     <cfRule type="cellIs" priority="86" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="313">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F18">
+  <conditionalFormatting sqref="C19:G19">
     <cfRule type="cellIs" priority="87" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="314">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F18">
+  <conditionalFormatting sqref="I41">
     <cfRule type="cellIs" priority="88" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="315">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12:F18">
+  <conditionalFormatting sqref="I41">
     <cfRule type="cellIs" priority="89" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="316">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37:E41">
+  <conditionalFormatting sqref="H40:H41">
     <cfRule type="cellIs" priority="90" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="317">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E13">
-    <cfRule type="cellIs" priority="92" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E18">
-    <cfRule type="cellIs" priority="93" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G18">
-    <cfRule type="cellIs" priority="94" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37:H39 H42:H45">
-    <cfRule type="cellIs" priority="95" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:D22">
-    <cfRule type="cellIs" priority="96" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:E22">
-    <cfRule type="cellIs" priority="97" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G21:G22">
-    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H22">
-    <cfRule type="cellIs" priority="99" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I21:I22">
-    <cfRule type="cellIs" priority="100" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" priority="101" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:G19">
-    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40:I41">
-    <cfRule type="cellIs" priority="104" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I40:I41">
-    <cfRule type="cellIs" priority="105" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40:H41">
-    <cfRule type="cellIs" priority="106" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15289,7 +15142,7 @@
   <dimension ref="B1:AMJ52"/>
   <sheetViews>
     <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15397,11 +15250,11 @@
       <c r="F9" s="299"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="302"/>
-      <c r="C10" s="302"/>
-      <c r="D10" s="302"/>
-      <c r="E10" s="302"/>
-      <c r="F10" s="302"/>
+      <c r="B10" s="303"/>
+      <c r="C10" s="303"/>
+      <c r="D10" s="303"/>
+      <c r="E10" s="303"/>
+      <c r="F10" s="303"/>
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="325" t="s">
@@ -15541,11 +15394,13 @@
       <c r="F25" s="299"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="302"/>
-      <c r="C26" s="302"/>
-      <c r="D26" s="302"/>
-      <c r="E26" s="302"/>
-      <c r="F26" s="302"/>
+      <c r="B26" s="303" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="303"/>
+      <c r="D26" s="303"/>
+      <c r="E26" s="303"/>
+      <c r="F26" s="303"/>
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="325" t="s">
@@ -15685,11 +15540,11 @@
       <c r="F41" s="299"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="302"/>
-      <c r="C42" s="302"/>
-      <c r="D42" s="302"/>
-      <c r="E42" s="302"/>
-      <c r="F42" s="302"/>
+      <c r="B42" s="303"/>
+      <c r="C42" s="303"/>
+      <c r="D42" s="303"/>
+      <c r="E42" s="303"/>
+      <c r="F42" s="303"/>
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="325" t="s">
@@ -15823,142 +15678,142 @@
     <mergeCell ref="B47:B48"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:AMJ3 H54:AMJ1048576 B2:B3 H11:AMJ14 H4:AMJ10 B20:F26 H16:AMJ31 B33:F42 G33:AMJ47 G2:G3 A54:G1048576 G11:G14 A4:G10 G16:G31 A52:AMJ53">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="318">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49:AMJ51">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="319">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:C30 B27">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="320">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="321">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:F19">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="322">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C14 B11">
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="323">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="324">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:F51">
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="325">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:C46 B43">
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="326">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="327">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="328">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="329">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="330">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="331">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="332">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:E16">
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="333">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="334">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:AMJ32">
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="335">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:E32">
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="336">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353">
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="337">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:AMJ48">
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354">
+    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="338">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:E48">
-    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355">
+    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="339">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F48">
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356">
+    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="340">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:AMJ15">
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357">
+    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="341">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358">
+    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="342">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359">
+    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="343">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360">
+    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="344">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361">
+    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="345">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15984,10 +15839,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:G57"/>
+  <dimension ref="B1:G58"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
+    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16055,11 +15910,11 @@
       <c r="F8" s="299"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="302"/>
-      <c r="C9" s="302"/>
-      <c r="D9" s="302"/>
-      <c r="E9" s="302"/>
-      <c r="F9" s="302"/>
+      <c r="B9" s="303"/>
+      <c r="C9" s="303"/>
+      <c r="D9" s="303"/>
+      <c r="E9" s="303"/>
+      <c r="F9" s="303"/>
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="337" t="s">
@@ -16138,28 +15993,30 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="326" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="332"/>
       <c r="D17" s="332"/>
       <c r="E17" s="332"/>
       <c r="F17" s="332"/>
     </row>
-    <row r="18" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="333" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="326" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="332"/>
+      <c r="D18" s="332"/>
+      <c r="E18" s="332"/>
+      <c r="F18" s="332"/>
+    </row>
+    <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="333" t="s">
         <v>206</v>
       </c>
-      <c r="C18" s="336"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="334"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="299"/>
-      <c r="C19" s="299"/>
-      <c r="D19" s="299"/>
-      <c r="E19" s="299"/>
-      <c r="F19" s="299"/>
+      <c r="C19" s="336"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="334"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="299"/>
@@ -16203,27 +16060,25 @@
       <c r="E25" s="299"/>
       <c r="F25" s="299"/>
     </row>
-    <row r="26" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="337" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="299"/>
+      <c r="C26" s="299"/>
+      <c r="D26" s="299"/>
+      <c r="E26" s="299"/>
+      <c r="F26" s="299"/>
+    </row>
+    <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="337" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="337"/>
-      <c r="D26" s="337"/>
-      <c r="E26" s="337"/>
-      <c r="F26" s="337"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="326" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="338"/>
-      <c r="D27" s="338"/>
-      <c r="E27" s="338"/>
-      <c r="F27" s="338"/>
+      <c r="C27" s="337"/>
+      <c r="D27" s="337"/>
+      <c r="E27" s="337"/>
+      <c r="F27" s="337"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="326" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="338"/>
       <c r="D28" s="338"/>
@@ -16232,55 +16087,55 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="326" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="338"/>
       <c r="D29" s="338"/>
       <c r="E29" s="338"/>
       <c r="F29" s="338"/>
     </row>
-    <row r="30" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="335"/>
-      <c r="C30" s="329" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="326" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="338"/>
+      <c r="D30" s="338"/>
+      <c r="E30" s="338"/>
+      <c r="F30" s="338"/>
+    </row>
+    <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="335"/>
+      <c r="C31" s="329" t="s">
         <v>204</v>
       </c>
-      <c r="D30" s="329" t="s">
+      <c r="D31" s="329" t="s">
         <v>201</v>
       </c>
-      <c r="E30" s="329" t="s">
+      <c r="E31" s="329" t="s">
         <v>202</v>
       </c>
-      <c r="F30" s="330" t="s">
+      <c r="F31" s="330" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="335"/>
-      <c r="C31" s="113" t="s">
+    <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="335"/>
+      <c r="C32" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="113" t="s">
+      <c r="D32" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="113" t="s">
+      <c r="E32" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="113" t="s">
+      <c r="F32" s="113" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="326" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="332"/>
-      <c r="D32" s="332"/>
-      <c r="E32" s="332"/>
-      <c r="F32" s="332"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="326" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="332"/>
       <c r="D33" s="332"/>
@@ -16289,28 +16144,30 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="326" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="332"/>
       <c r="D34" s="332"/>
       <c r="E34" s="332"/>
       <c r="F34" s="332"/>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="339" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="326" t="n">
+        <v>3</v>
+      </c>
+      <c r="C35" s="332"/>
+      <c r="D35" s="332"/>
+      <c r="E35" s="332"/>
+      <c r="F35" s="332"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="339" t="s">
         <v>207</v>
       </c>
-      <c r="C35" s="339"/>
-      <c r="D35" s="339"/>
-      <c r="E35" s="339"/>
-      <c r="F35" s="339"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="299"/>
-      <c r="C36" s="299"/>
-      <c r="D36" s="299"/>
-      <c r="E36" s="299"/>
-      <c r="F36" s="299"/>
+      <c r="C36" s="339"/>
+      <c r="D36" s="339"/>
+      <c r="E36" s="339"/>
+      <c r="F36" s="339"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="299"/>
@@ -16348,20 +16205,20 @@
       <c r="F41" s="299"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="340"/>
-      <c r="C42" s="340"/>
-      <c r="D42" s="340"/>
-      <c r="E42" s="340"/>
-      <c r="F42" s="340"/>
-    </row>
-    <row r="43" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="299"/>
-      <c r="C43" s="299"/>
-      <c r="D43" s="299"/>
-      <c r="E43" s="299"/>
-      <c r="F43" s="299"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="299"/>
+      <c r="C42" s="299"/>
+      <c r="D42" s="299"/>
+      <c r="E42" s="299"/>
+      <c r="F42" s="299"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="340"/>
+      <c r="C43" s="340"/>
+      <c r="D43" s="340"/>
+      <c r="E43" s="340"/>
+      <c r="F43" s="340"/>
+    </row>
+    <row r="44" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="299"/>
       <c r="C44" s="299"/>
       <c r="D44" s="299"/>
@@ -16410,37 +16267,37 @@
       <c r="E50" s="299"/>
       <c r="F50" s="299"/>
     </row>
-    <row r="51" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="322" t="s">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="299"/>
+      <c r="C51" s="299"/>
+      <c r="D51" s="299"/>
+      <c r="E51" s="299"/>
+      <c r="F51" s="299"/>
+    </row>
+    <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="322" t="s">
         <v>208</v>
       </c>
-      <c r="C51" s="95"/>
-      <c r="D51" s="323"/>
-      <c r="E51" s="323"/>
-      <c r="F51" s="324"/>
-    </row>
-    <row r="52" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="151"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="154"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="296" t="s">
+      <c r="C52" s="95"/>
+      <c r="D52" s="323"/>
+      <c r="E52" s="323"/>
+      <c r="F52" s="324"/>
+    </row>
+    <row r="53" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="151"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="154"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B54" s="297" t="s">
         <v>209</v>
       </c>
-      <c r="C53" s="296"/>
-      <c r="D53" s="296"/>
-      <c r="E53" s="296"/>
-      <c r="F53" s="296"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="299"/>
-      <c r="C54" s="299"/>
-      <c r="D54" s="299"/>
-      <c r="E54" s="299"/>
-      <c r="F54" s="299"/>
+      <c r="C54" s="297"/>
+      <c r="D54" s="297"/>
+      <c r="E54" s="297"/>
+      <c r="F54" s="297"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="299"/>
@@ -16456,12 +16313,19 @@
       <c r="E56" s="299"/>
       <c r="F56" s="299"/>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="145"/>
-      <c r="C57" s="146"/>
-      <c r="D57" s="146"/>
-      <c r="E57" s="146"/>
-      <c r="F57" s="341"/>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="299"/>
+      <c r="C57" s="299"/>
+      <c r="D57" s="299"/>
+      <c r="E57" s="299"/>
+      <c r="F57" s="299"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="145"/>
+      <c r="C58" s="146"/>
+      <c r="D58" s="146"/>
+      <c r="E58" s="146"/>
+      <c r="F58" s="341"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -16477,7 +16341,6 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B19:F19"/>
     <mergeCell ref="B20:F20"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B22:F22"/>
@@ -16485,11 +16348,11 @@
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B26:F26"/>
-    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="B27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="B38:F38"/>
@@ -16505,93 +16368,94 @@
     <mergeCell ref="B48:F48"/>
     <mergeCell ref="B49:F49"/>
     <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B51:F51"/>
     <mergeCell ref="B54:F54"/>
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B57:F57"/>
   </mergeCells>
-  <conditionalFormatting sqref="H10:AMJ14 B38:B42 B50:F50 H52:AMJ52 H32:AMJ50 B36:F37 B35 B11:C13 B10 H61:AMJ1048576 H51:AMJ51 H2:AMJ9 H16:AMJ30 B16:F25 G53:AMJ56 B54:B56 G10:G14 D52:G52 G32:G50 A61:G1048576 A51:G51 A2:G9 G16:G30 A57:AMJ60">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362">
+  <conditionalFormatting sqref="H10:AMJ14 B39:B43 B51:F51 H53:AMJ53 H33:AMJ51 B37:F38 B36 B11:C13 B10 H62:AMJ1048576 H52:AMJ52 H2:AMJ9 H18:AMJ31 G54:AMJ57 B55:B57 G10:G14 D53:G53 G33:G51 A62:G1048576 A52:G52 A2:G9 G18:G31 A58:AMJ61 B18:F26 B16:AMJ17">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="346">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="363">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27:C29 B26 B32:F34">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="364">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:C30">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="365">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43:B49">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="366">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="367">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="368">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="347">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:C30 B27 B33:F35">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="348">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:C31">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="349">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44:B50">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="350">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="351">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="352">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="369">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="353">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="370">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="354">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="371">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31:AMJ31">
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="372">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31:E31">
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="373">
-      <formula>"*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F31">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="374">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="355">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32:AMJ32">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="356">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:E32">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="357">
+      <formula>"*"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="358">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:AMJ15">
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="375">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="359">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:E15">
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="376">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="360">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="377">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="361">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B11:B13 B16:F17 B27:B29 B32:F34" type="custom">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B11:B13 B16:F18 B28:B30 B33:F35" type="custom">
       <formula1>OR(ISNUMBER(B32),B32="*")</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -16615,7 +16479,7 @@
   <dimension ref="B1:I61"/>
   <sheetViews>
     <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17235,8 +17099,8 @@
     <mergeCell ref="B59:H59"/>
     <mergeCell ref="B60:H60"/>
   </mergeCells>
-  <conditionalFormatting sqref="J2:AMJ2 B2 A3:AMJ1048576 I2">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="378">
+  <conditionalFormatting sqref="I2:AMJ2 B2 A3:AMJ1048576">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="362">
       <formula>"*"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
AE-207:  added laatija to energiatodistus pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="211">
   <si>
     <t xml:space="preserve">ENERGIATODISTUS 2018</t>
   </si>
@@ -1597,7 +1597,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00000"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
-    <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
+    <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
     <numFmt numFmtId="168" formatCode="0%"/>
     <numFmt numFmtId="169" formatCode="@"/>
     <numFmt numFmtId="170" formatCode="0"/>
@@ -2374,7 +2374,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2497,7 +2497,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6253,9 +6253,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6269,7 +6269,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="758520" cy="215280"/>
+          <a:ext cx="758160" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6290,9 +6290,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>148320</xdr:colOff>
+      <xdr:colOff>147960</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6306,7 +6306,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1101960" cy="215280"/>
+          <a:ext cx="1101600" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6327,9 +6327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>21600</xdr:colOff>
+      <xdr:colOff>21240</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6343,7 +6343,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1408680" cy="215280"/>
+          <a:ext cx="1408320" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6364,9 +6364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>345600</xdr:colOff>
+      <xdr:colOff>345240</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6380,7 +6380,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1732680" cy="215280"/>
+          <a:ext cx="1732320" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6401,9 +6401,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>218880</xdr:colOff>
+      <xdr:colOff>218520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>275760</xdr:rowOff>
+      <xdr:rowOff>275400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6417,7 +6417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2039760" cy="228240"/>
+          <a:ext cx="2039400" cy="227880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6438,9 +6438,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>162000</xdr:colOff>
+      <xdr:colOff>161640</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>262800</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6454,7 +6454,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2376000" cy="215280"/>
+          <a:ext cx="2375640" cy="214920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6475,9 +6475,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
+      <xdr:colOff>101880</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>262440</xdr:rowOff>
+      <xdr:rowOff>262080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6487,7 +6487,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530040"/>
-          <a:ext cx="2688840" cy="214200"/>
+          <a:ext cx="2688480" cy="213840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6856,9 +6856,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>301680</xdr:colOff>
+      <xdr:colOff>301320</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>102240</xdr:rowOff>
+      <xdr:rowOff>101880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6868,7 +6868,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6987960" cy="10557720"/>
+          <a:ext cx="6987600" cy="10557360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6996,9 +6996,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>426240</xdr:colOff>
+      <xdr:colOff>425880</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>296280</xdr:rowOff>
+      <xdr:rowOff>295920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7012,7 +7012,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5087160" y="5274720"/>
-          <a:ext cx="1126440" cy="259560"/>
+          <a:ext cx="1126080" cy="259200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7038,9 +7038,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>148680</xdr:colOff>
+      <xdr:colOff>148320</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7050,7 +7050,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="201240" y="10549800"/>
-          <a:ext cx="7023240" cy="257760"/>
+          <a:ext cx="7022880" cy="257400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7109,9 +7109,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1013400</xdr:colOff>
+      <xdr:colOff>1013040</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7121,7 +7121,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="396000" y="10928880"/>
-          <a:ext cx="7090560" cy="264240"/>
+          <a:ext cx="7090200" cy="263880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7180,9 +7180,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1017000</xdr:colOff>
+      <xdr:colOff>1016640</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7192,7 +7192,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="290520" y="11094480"/>
-          <a:ext cx="7050240" cy="259200"/>
+          <a:ext cx="7049880" cy="258840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7251,9 +7251,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>33480</xdr:colOff>
+      <xdr:colOff>33120</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7263,7 +7263,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="241920" y="9930960"/>
-          <a:ext cx="6889320" cy="258480"/>
+          <a:ext cx="6888960" cy="258120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7322,9 +7322,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>52200</xdr:colOff>
+      <xdr:colOff>51840</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7334,7 +7334,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="170640" y="10200240"/>
-          <a:ext cx="6985800" cy="359280"/>
+          <a:ext cx="6985440" cy="358920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7393,9 +7393,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>61560</xdr:colOff>
+      <xdr:colOff>61200</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7405,7 +7405,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="163440" y="10335960"/>
-          <a:ext cx="6994800" cy="370440"/>
+          <a:ext cx="6994440" cy="370080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7464,9 +7464,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>66600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7476,7 +7476,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="90720" y="9993600"/>
-          <a:ext cx="7035120" cy="370440"/>
+          <a:ext cx="7034760" cy="370080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7531,8 +7531,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ51"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M32" activeCellId="0" sqref="M32"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8755,9 +8755,7 @@
     </row>
     <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
-      <c r="B42" s="75" t="s">
-        <v>14</v>
-      </c>
+      <c r="B42" s="75"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -9075,7 +9073,7 @@
   </sheetPr>
   <dimension ref="B1:AA65"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -11057,7 +11055,7 @@
   </sheetPr>
   <dimension ref="B2:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -12416,7 +12414,7 @@
   </sheetPr>
   <dimension ref="B2:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E74" activeCellId="0" sqref="E74"/>
     </sheetView>
   </sheetViews>
@@ -13786,7 +13784,7 @@
   </sheetPr>
   <dimension ref="B2:AMJ55"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
@@ -15121,7 +15119,7 @@
   </sheetPr>
   <dimension ref="B1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -15821,7 +15819,7 @@
   </sheetPr>
   <dimension ref="B1:G58"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -16458,7 +16456,7 @@
   </sheetPr>
   <dimension ref="B1:I61"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AE-231 implement energiatodistus pdf first page checkbox handling
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -68,16 +68,16 @@
     <t xml:space="preserve">Energiatodistus on laadittu</t>
   </si>
   <si>
-    <t xml:space="preserve"> Uudelle rakennukselle rakennuslupaa haettaessa</t>
+    <t xml:space="preserve">☐ Uudelle rakennukselle rakennuslupaa haettaessa</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> Uudelle rakennukselle käyttöönottovaiheessa    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Olemassa olevalle rakennukselle, havainnointikäynnin päivämäärä:</t>
+    <t xml:space="preserve">☐ Uudelle rakennukselle käyttöönottovaiheessa    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">☐ Olemassa olevalle rakennukselle, havainnointikäynnin päivämäärä:</t>
   </si>
   <si>
     <t xml:space="preserve">Energiatehokkuusluokka </t>
@@ -7620,8 +7620,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F54" activeCellId="0" sqref="F54"/>
+    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
AE-271 include uusiutuva polttoaine to käytettävät energiamuodot -table in pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="208">
   <si>
     <t xml:space="preserve">ENERGIATODISTUS 2018</t>
   </si>
@@ -11135,7 +11135,7 @@
   </sheetPr>
   <dimension ref="B2:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
     </sheetView>
   </sheetViews>
@@ -12473,8 +12473,8 @@
   </sheetPr>
   <dimension ref="B2:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I55" activeCellId="0" sqref="I55"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12729,7 +12729,9 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="165"/>
-      <c r="C21" s="265"/>
+      <c r="C21" s="265" t="s">
+        <v>36</v>
+      </c>
       <c r="D21" s="237"/>
       <c r="E21" s="193"/>
       <c r="F21" s="237"/>

</xml_diff>

<commit_message>
AE-271 replace red placeholder with blue value in energiatodistus xlsx template
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -1598,7 +1598,7 @@
     <numFmt numFmtId="174" formatCode="@"/>
     <numFmt numFmtId="175" formatCode="0"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1866,14 +1866,6 @@
       <b val="true"/>
       <sz val="8"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2199,7 +2191,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="373">
+  <cellXfs count="372">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3292,10 +3284,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -3308,15 +3296,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="39" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="169" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -3568,7 +3556,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -12473,8 +12461,8 @@
   </sheetPr>
   <dimension ref="B2:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12957,7 +12945,7 @@
       <c r="D43" s="166"/>
       <c r="E43" s="237"/>
       <c r="F43" s="237"/>
-      <c r="G43" s="273" t="s">
+      <c r="G43" s="189" t="s">
         <v>32</v>
       </c>
     </row>
@@ -13083,7 +13071,7 @@
       <c r="D55" s="166"/>
       <c r="E55" s="237"/>
       <c r="F55" s="237"/>
-      <c r="G55" s="274"/>
+      <c r="G55" s="273"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="165"/>
@@ -13103,35 +13091,35 @@
       <c r="D57" s="166"/>
       <c r="E57" s="237"/>
       <c r="F57" s="237"/>
-      <c r="G57" s="274"/>
+      <c r="G57" s="273"/>
     </row>
     <row r="58" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="165"/>
       <c r="C58" s="166"/>
       <c r="D58" s="166"/>
-      <c r="E58" s="275"/>
-      <c r="F58" s="275"/>
-      <c r="G58" s="276"/>
+      <c r="E58" s="274"/>
+      <c r="F58" s="274"/>
+      <c r="G58" s="275"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="165"/>
       <c r="C59" s="224" t="s">
         <v>158</v>
       </c>
-      <c r="D59" s="277"/>
-      <c r="E59" s="278"/>
-      <c r="F59" s="278"/>
-      <c r="G59" s="276"/>
+      <c r="D59" s="276"/>
+      <c r="E59" s="277"/>
+      <c r="F59" s="277"/>
+      <c r="G59" s="275"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="165"/>
       <c r="C60" s="224" t="s">
         <v>159</v>
       </c>
-      <c r="D60" s="277"/>
-      <c r="E60" s="279"/>
-      <c r="F60" s="279"/>
-      <c r="G60" s="280"/>
+      <c r="D60" s="276"/>
+      <c r="E60" s="278"/>
+      <c r="F60" s="278"/>
+      <c r="G60" s="279"/>
     </row>
     <row r="61" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="165"/>
@@ -13187,7 +13175,7 @@
       <c r="D66" s="166"/>
       <c r="E66" s="237"/>
       <c r="F66" s="237"/>
-      <c r="G66" s="274"/>
+      <c r="G66" s="273"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="165"/>
@@ -13197,7 +13185,7 @@
       <c r="D67" s="166"/>
       <c r="E67" s="237"/>
       <c r="F67" s="237"/>
-      <c r="G67" s="274"/>
+      <c r="G67" s="273"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="165"/>
@@ -13207,7 +13195,7 @@
       <c r="D68" s="166"/>
       <c r="E68" s="237"/>
       <c r="F68" s="237"/>
-      <c r="G68" s="274"/>
+      <c r="G68" s="273"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="165"/>
@@ -13217,7 +13205,7 @@
       <c r="D69" s="166"/>
       <c r="E69" s="237"/>
       <c r="F69" s="237"/>
-      <c r="G69" s="274"/>
+      <c r="G69" s="273"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="165"/>
@@ -13227,7 +13215,7 @@
       <c r="D70" s="166"/>
       <c r="E70" s="237"/>
       <c r="F70" s="237"/>
-      <c r="G70" s="274"/>
+      <c r="G70" s="273"/>
     </row>
     <row r="71" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="165"/>
@@ -13261,9 +13249,9 @@
         <v>163</v>
       </c>
       <c r="D74" s="166"/>
-      <c r="E74" s="281"/>
-      <c r="F74" s="281"/>
-      <c r="G74" s="281"/>
+      <c r="E74" s="280"/>
+      <c r="F74" s="280"/>
+      <c r="G74" s="280"/>
     </row>
     <row r="75" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="241"/>
@@ -13271,7 +13259,7 @@
       <c r="D75" s="178"/>
       <c r="E75" s="241"/>
       <c r="F75" s="178"/>
-      <c r="G75" s="282"/>
+      <c r="G75" s="281"/>
     </row>
     <row r="76" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -13789,18 +13777,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="978" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" s="283" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="284"/>
-      <c r="C2" s="285" t="s">
+    <row r="2" s="282" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="283"/>
+      <c r="C2" s="284" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="285"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="287"/>
+      <c r="D2" s="284"/>
+      <c r="E2" s="285"/>
+      <c r="F2" s="285"/>
+      <c r="G2" s="285"/>
+      <c r="H2" s="285"/>
+      <c r="I2" s="285"/>
+      <c r="J2" s="286"/>
       <c r="AKP2" s="0"/>
       <c r="AKQ2" s="0"/>
       <c r="AKR2" s="0"/>
@@ -13851,16 +13839,16 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="100"/>
-      <c r="C3" s="288" t="s">
+      <c r="C3" s="287" t="s">
         <v>165</v>
       </c>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
+      <c r="D3" s="287"/>
+      <c r="E3" s="287"/>
+      <c r="F3" s="287"/>
+      <c r="G3" s="287"/>
+      <c r="H3" s="287"/>
+      <c r="I3" s="287"/>
+      <c r="J3" s="287"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="100"/>
@@ -13903,11 +13891,11 @@
       <c r="C7" s="105"/>
       <c r="D7" s="106"/>
       <c r="E7" s="106"/>
-      <c r="F7" s="289"/>
+      <c r="F7" s="288"/>
       <c r="G7" s="106"/>
       <c r="H7" s="106"/>
       <c r="I7" s="106"/>
-      <c r="J7" s="290"/>
+      <c r="J7" s="289"/>
       <c r="K7" s="108"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13932,22 +13920,22 @@
       <c r="I9" s="110"/>
       <c r="J9" s="111"/>
     </row>
-    <row r="10" s="283" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="291"/>
-      <c r="C10" s="292" t="s">
+    <row r="10" s="282" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="290"/>
+      <c r="C10" s="291" t="s">
         <v>167</v>
       </c>
-      <c r="D10" s="293"/>
-      <c r="E10" s="294"/>
-      <c r="F10" s="295"/>
-      <c r="G10" s="296"/>
-      <c r="H10" s="297" t="s">
+      <c r="D10" s="292"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="294"/>
+      <c r="G10" s="295"/>
+      <c r="H10" s="296" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="297" t="s">
+      <c r="I10" s="296" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="297"/>
+      <c r="J10" s="296"/>
       <c r="AKP10" s="0"/>
       <c r="AKQ10" s="0"/>
       <c r="AKR10" s="0"/>
@@ -14000,11 +13988,11 @@
       <c r="B11" s="100"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="298"/>
+      <c r="E11" s="297"/>
       <c r="F11" s="46"/>
       <c r="G11" s="122"/>
       <c r="H11" s="118"/>
-      <c r="I11" s="299"/>
+      <c r="I11" s="298"/>
       <c r="J11" s="122"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14013,23 +14001,23 @@
         <v>168</v>
       </c>
       <c r="D12" s="103"/>
-      <c r="E12" s="300"/>
+      <c r="E12" s="299"/>
       <c r="F12" s="75"/>
-      <c r="G12" s="301"/>
+      <c r="G12" s="300"/>
       <c r="H12" s="237"/>
       <c r="I12" s="126"/>
-      <c r="J12" s="302"/>
+      <c r="J12" s="301"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="100"/>
       <c r="C13" s="103"/>
       <c r="D13" s="103"/>
-      <c r="E13" s="300"/>
+      <c r="E13" s="299"/>
       <c r="F13" s="75"/>
-      <c r="G13" s="301"/>
+      <c r="G13" s="300"/>
       <c r="H13" s="237"/>
       <c r="I13" s="126"/>
-      <c r="J13" s="302"/>
+      <c r="J13" s="301"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="100"/>
@@ -14037,60 +14025,60 @@
         <v>169</v>
       </c>
       <c r="D14" s="103"/>
-      <c r="E14" s="300"/>
+      <c r="E14" s="299"/>
       <c r="F14" s="75"/>
-      <c r="G14" s="301"/>
+      <c r="G14" s="300"/>
       <c r="H14" s="237"/>
       <c r="I14" s="126"/>
-      <c r="J14" s="302"/>
+      <c r="J14" s="301"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="100"/>
       <c r="C15" s="103"/>
       <c r="D15" s="103"/>
-      <c r="E15" s="300"/>
+      <c r="E15" s="299"/>
       <c r="F15" s="75"/>
-      <c r="G15" s="301"/>
+      <c r="G15" s="300"/>
       <c r="H15" s="237"/>
       <c r="I15" s="126"/>
-      <c r="J15" s="302"/>
+      <c r="J15" s="301"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="100"/>
-      <c r="C16" s="303" t="s">
+      <c r="C16" s="302" t="s">
         <v>170</v>
       </c>
       <c r="D16" s="103"/>
-      <c r="E16" s="300"/>
+      <c r="E16" s="299"/>
       <c r="F16" s="75"/>
-      <c r="G16" s="301"/>
+      <c r="G16" s="300"/>
       <c r="H16" s="237"/>
       <c r="I16" s="126"/>
-      <c r="J16" s="302"/>
+      <c r="J16" s="301"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="100"/>
-      <c r="C17" s="303" t="s">
+      <c r="C17" s="302" t="s">
         <v>171</v>
       </c>
       <c r="D17" s="103"/>
-      <c r="E17" s="300"/>
+      <c r="E17" s="299"/>
       <c r="F17" s="75"/>
-      <c r="G17" s="301"/>
+      <c r="G17" s="300"/>
       <c r="H17" s="237"/>
       <c r="I17" s="126"/>
-      <c r="J17" s="302"/>
+      <c r="J17" s="301"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="100"/>
-      <c r="C18" s="303"/>
+      <c r="C18" s="302"/>
       <c r="D18" s="103"/>
-      <c r="E18" s="300"/>
+      <c r="E18" s="299"/>
       <c r="F18" s="75"/>
-      <c r="G18" s="300"/>
+      <c r="G18" s="299"/>
       <c r="H18" s="237"/>
       <c r="I18" s="126"/>
-      <c r="J18" s="302"/>
+      <c r="J18" s="301"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="100"/>
@@ -14103,41 +14091,41 @@
       <c r="G19" s="103"/>
       <c r="H19" s="237"/>
       <c r="I19" s="126"/>
-      <c r="J19" s="302"/>
+      <c r="J19" s="301"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="109"/>
-      <c r="C20" s="304"/>
-      <c r="D20" s="304"/>
-      <c r="E20" s="304"/>
-      <c r="F20" s="304"/>
-      <c r="G20" s="304"/>
-      <c r="H20" s="305"/>
-      <c r="I20" s="306"/>
-      <c r="J20" s="307"/>
-    </row>
-    <row r="21" s="283" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="291"/>
-      <c r="C21" s="292" t="s">
+      <c r="C20" s="303"/>
+      <c r="D20" s="303"/>
+      <c r="E20" s="303"/>
+      <c r="F20" s="303"/>
+      <c r="G20" s="303"/>
+      <c r="H20" s="304"/>
+      <c r="I20" s="305"/>
+      <c r="J20" s="306"/>
+    </row>
+    <row r="21" s="282" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="290"/>
+      <c r="C21" s="291" t="s">
         <v>172</v>
       </c>
-      <c r="D21" s="292"/>
-      <c r="E21" s="308" t="s">
+      <c r="D21" s="291"/>
+      <c r="E21" s="307" t="s">
         <v>173</v>
       </c>
-      <c r="F21" s="309" t="s">
+      <c r="F21" s="308" t="s">
         <v>174</v>
       </c>
-      <c r="G21" s="308" t="s">
+      <c r="G21" s="307" t="s">
         <v>175</v>
       </c>
-      <c r="H21" s="309" t="s">
+      <c r="H21" s="308" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="309" t="s">
+      <c r="I21" s="308" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="309"/>
+      <c r="J21" s="308"/>
       <c r="AKP21" s="0"/>
       <c r="AKQ21" s="0"/>
       <c r="AKR21" s="0"/>
@@ -14188,14 +14176,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="94"/>
-      <c r="C22" s="310"/>
-      <c r="D22" s="310"/>
-      <c r="E22" s="311"/>
-      <c r="F22" s="312"/>
-      <c r="G22" s="313"/>
-      <c r="H22" s="314"/>
-      <c r="I22" s="315"/>
-      <c r="J22" s="316"/>
+      <c r="C22" s="309"/>
+      <c r="D22" s="309"/>
+      <c r="E22" s="310"/>
+      <c r="F22" s="311"/>
+      <c r="G22" s="312"/>
+      <c r="H22" s="313"/>
+      <c r="I22" s="314"/>
+      <c r="J22" s="315"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="100"/>
@@ -14204,15 +14192,15 @@
       </c>
       <c r="D23" s="103"/>
       <c r="E23" s="237"/>
-      <c r="F23" s="317" t="s">
+      <c r="F23" s="316" t="s">
         <v>177</v>
       </c>
-      <c r="G23" s="318" t="n">
+      <c r="G23" s="317" t="n">
         <v>10</v>
       </c>
       <c r="H23" s="126"/>
       <c r="I23" s="126"/>
-      <c r="J23" s="302"/>
+      <c r="J23" s="301"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="100"/>
@@ -14221,15 +14209,15 @@
       </c>
       <c r="D24" s="103"/>
       <c r="E24" s="237"/>
-      <c r="F24" s="317" t="s">
+      <c r="F24" s="316" t="s">
         <v>179</v>
       </c>
-      <c r="G24" s="318" t="n">
+      <c r="G24" s="317" t="n">
         <v>1300</v>
       </c>
       <c r="H24" s="126"/>
       <c r="I24" s="126"/>
-      <c r="J24" s="302"/>
+      <c r="J24" s="301"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="100"/>
@@ -14238,15 +14226,15 @@
       </c>
       <c r="D25" s="103"/>
       <c r="E25" s="237"/>
-      <c r="F25" s="317" t="s">
+      <c r="F25" s="316" t="s">
         <v>179</v>
       </c>
-      <c r="G25" s="318" t="n">
+      <c r="G25" s="317" t="n">
         <v>1700</v>
       </c>
       <c r="H25" s="126"/>
       <c r="I25" s="126"/>
-      <c r="J25" s="302"/>
+      <c r="J25" s="301"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="100"/>
@@ -14255,126 +14243,126 @@
       </c>
       <c r="D26" s="103"/>
       <c r="E26" s="237"/>
-      <c r="F26" s="317" t="s">
+      <c r="F26" s="316" t="s">
         <v>182</v>
       </c>
-      <c r="G26" s="318" t="n">
+      <c r="G26" s="317" t="n">
         <v>4.7</v>
       </c>
       <c r="H26" s="126"/>
       <c r="I26" s="126"/>
-      <c r="J26" s="302"/>
+      <c r="J26" s="301"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="100"/>
-      <c r="C27" s="319"/>
-      <c r="D27" s="319"/>
+      <c r="C27" s="318"/>
+      <c r="D27" s="318"/>
       <c r="E27" s="237"/>
-      <c r="F27" s="320"/>
+      <c r="F27" s="319"/>
       <c r="G27" s="193"/>
       <c r="H27" s="124"/>
       <c r="I27" s="126"/>
-      <c r="J27" s="321"/>
+      <c r="J27" s="320"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="100"/>
-      <c r="C28" s="319"/>
-      <c r="D28" s="319"/>
+      <c r="C28" s="318"/>
+      <c r="D28" s="318"/>
       <c r="E28" s="237"/>
-      <c r="F28" s="320"/>
+      <c r="F28" s="319"/>
       <c r="G28" s="193"/>
       <c r="H28" s="124"/>
       <c r="I28" s="126"/>
-      <c r="J28" s="321"/>
+      <c r="J28" s="320"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="100"/>
-      <c r="C29" s="322" t="s">
+      <c r="C29" s="321" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="322"/>
+      <c r="D29" s="321"/>
       <c r="E29" s="237"/>
-      <c r="F29" s="323"/>
+      <c r="F29" s="322"/>
       <c r="G29" s="205"/>
       <c r="H29" s="124"/>
       <c r="I29" s="126"/>
-      <c r="J29" s="302"/>
+      <c r="J29" s="301"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="100"/>
-      <c r="C30" s="322"/>
-      <c r="D30" s="322"/>
+      <c r="C30" s="321"/>
+      <c r="D30" s="321"/>
       <c r="E30" s="237"/>
-      <c r="F30" s="323"/>
+      <c r="F30" s="322"/>
       <c r="G30" s="205"/>
       <c r="H30" s="124"/>
       <c r="I30" s="126"/>
-      <c r="J30" s="302"/>
+      <c r="J30" s="301"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="100"/>
-      <c r="C31" s="322"/>
-      <c r="D31" s="322"/>
+      <c r="C31" s="321"/>
+      <c r="D31" s="321"/>
       <c r="E31" s="205"/>
-      <c r="F31" s="323"/>
+      <c r="F31" s="322"/>
       <c r="G31" s="205"/>
-      <c r="H31" s="324"/>
-      <c r="I31" s="325"/>
-      <c r="J31" s="302"/>
+      <c r="H31" s="323"/>
+      <c r="I31" s="324"/>
+      <c r="J31" s="301"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="100"/>
-      <c r="C32" s="322"/>
-      <c r="D32" s="322"/>
+      <c r="C32" s="321"/>
+      <c r="D32" s="321"/>
       <c r="E32" s="205"/>
-      <c r="F32" s="323"/>
+      <c r="F32" s="322"/>
       <c r="G32" s="205"/>
-      <c r="H32" s="324"/>
-      <c r="I32" s="325"/>
-      <c r="J32" s="302"/>
+      <c r="H32" s="323"/>
+      <c r="I32" s="324"/>
+      <c r="J32" s="301"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="100"/>
-      <c r="C33" s="326"/>
-      <c r="D33" s="326"/>
+      <c r="C33" s="325"/>
+      <c r="D33" s="325"/>
       <c r="E33" s="205"/>
-      <c r="F33" s="323"/>
+      <c r="F33" s="322"/>
       <c r="G33" s="205"/>
-      <c r="H33" s="324"/>
-      <c r="I33" s="325"/>
-      <c r="J33" s="302"/>
+      <c r="H33" s="323"/>
+      <c r="I33" s="324"/>
+      <c r="J33" s="301"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="109"/>
-      <c r="C34" s="327"/>
-      <c r="D34" s="327"/>
+      <c r="C34" s="326"/>
+      <c r="D34" s="326"/>
       <c r="E34" s="211"/>
-      <c r="F34" s="328"/>
+      <c r="F34" s="327"/>
       <c r="G34" s="211"/>
-      <c r="H34" s="329"/>
-      <c r="I34" s="330"/>
-      <c r="J34" s="307"/>
+      <c r="H34" s="328"/>
+      <c r="I34" s="329"/>
+      <c r="J34" s="306"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="100"/>
-      <c r="C35" s="292" t="s">
+      <c r="C35" s="291" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="292"/>
-      <c r="E35" s="300"/>
+      <c r="D35" s="291"/>
+      <c r="E35" s="299"/>
       <c r="F35" s="75"/>
-      <c r="G35" s="300"/>
-      <c r="H35" s="331"/>
-      <c r="I35" s="332"/>
-      <c r="J35" s="302"/>
+      <c r="G35" s="299"/>
+      <c r="H35" s="330"/>
+      <c r="I35" s="331"/>
+      <c r="J35" s="301"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="100"/>
-      <c r="C36" s="292"/>
-      <c r="D36" s="292"/>
-      <c r="E36" s="300"/>
+      <c r="C36" s="291"/>
+      <c r="D36" s="291"/>
+      <c r="E36" s="299"/>
       <c r="F36" s="75"/>
-      <c r="G36" s="300"/>
+      <c r="G36" s="299"/>
       <c r="H36" s="115" t="s">
         <v>30</v>
       </c>
@@ -14385,14 +14373,14 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="94"/>
-      <c r="C37" s="333"/>
-      <c r="D37" s="333"/>
-      <c r="E37" s="334"/>
-      <c r="F37" s="335"/>
-      <c r="G37" s="335"/>
-      <c r="H37" s="336"/>
-      <c r="I37" s="337"/>
-      <c r="J37" s="338"/>
+      <c r="C37" s="332"/>
+      <c r="D37" s="332"/>
+      <c r="E37" s="333"/>
+      <c r="F37" s="334"/>
+      <c r="G37" s="334"/>
+      <c r="H37" s="335"/>
+      <c r="I37" s="336"/>
+      <c r="J37" s="337"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="100"/>
@@ -14400,23 +14388,23 @@
         <v>185</v>
       </c>
       <c r="D38" s="30"/>
-      <c r="E38" s="339"/>
-      <c r="F38" s="340"/>
-      <c r="G38" s="340"/>
+      <c r="E38" s="338"/>
+      <c r="F38" s="339"/>
+      <c r="G38" s="339"/>
       <c r="H38" s="237"/>
       <c r="I38" s="126"/>
-      <c r="J38" s="302"/>
+      <c r="J38" s="301"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="100"/>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
-      <c r="E39" s="339"/>
-      <c r="F39" s="340"/>
-      <c r="G39" s="340"/>
+      <c r="E39" s="338"/>
+      <c r="F39" s="339"/>
+      <c r="G39" s="339"/>
       <c r="H39" s="237"/>
-      <c r="I39" s="341"/>
-      <c r="J39" s="302"/>
+      <c r="I39" s="340"/>
+      <c r="J39" s="301"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="100"/>
@@ -14424,23 +14412,23 @@
         <v>186</v>
       </c>
       <c r="D40" s="30"/>
-      <c r="E40" s="339"/>
-      <c r="F40" s="340"/>
-      <c r="G40" s="340"/>
+      <c r="E40" s="338"/>
+      <c r="F40" s="339"/>
+      <c r="G40" s="339"/>
       <c r="H40" s="237"/>
       <c r="I40" s="126"/>
-      <c r="J40" s="302"/>
+      <c r="J40" s="301"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="100"/>
       <c r="C41" s="30"/>
       <c r="D41" s="30"/>
-      <c r="E41" s="339"/>
-      <c r="F41" s="340"/>
-      <c r="G41" s="340"/>
+      <c r="E41" s="338"/>
+      <c r="F41" s="339"/>
+      <c r="G41" s="339"/>
       <c r="H41" s="237"/>
-      <c r="I41" s="341"/>
-      <c r="J41" s="302"/>
+      <c r="I41" s="340"/>
+      <c r="J41" s="301"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="100"/>
@@ -14448,23 +14436,23 @@
         <v>187</v>
       </c>
       <c r="D42" s="30"/>
-      <c r="E42" s="339"/>
-      <c r="F42" s="340"/>
-      <c r="G42" s="340"/>
+      <c r="E42" s="338"/>
+      <c r="F42" s="339"/>
+      <c r="G42" s="339"/>
       <c r="H42" s="237"/>
       <c r="I42" s="126"/>
-      <c r="J42" s="302"/>
+      <c r="J42" s="301"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="100"/>
       <c r="C43" s="30"/>
       <c r="D43" s="30"/>
-      <c r="E43" s="339"/>
-      <c r="F43" s="340"/>
-      <c r="G43" s="340"/>
+      <c r="E43" s="338"/>
+      <c r="F43" s="339"/>
+      <c r="G43" s="339"/>
       <c r="H43" s="237"/>
-      <c r="I43" s="341"/>
-      <c r="J43" s="302"/>
+      <c r="I43" s="340"/>
+      <c r="J43" s="301"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="100"/>
@@ -14472,23 +14460,23 @@
         <v>147</v>
       </c>
       <c r="D44" s="30"/>
-      <c r="E44" s="339"/>
-      <c r="F44" s="340"/>
-      <c r="G44" s="340"/>
+      <c r="E44" s="338"/>
+      <c r="F44" s="339"/>
+      <c r="G44" s="339"/>
       <c r="H44" s="237"/>
       <c r="I44" s="126"/>
-      <c r="J44" s="302"/>
+      <c r="J44" s="301"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="100"/>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
-      <c r="E45" s="339"/>
-      <c r="F45" s="340"/>
-      <c r="G45" s="340"/>
+      <c r="E45" s="338"/>
+      <c r="F45" s="339"/>
+      <c r="G45" s="339"/>
       <c r="H45" s="237"/>
-      <c r="I45" s="341"/>
-      <c r="J45" s="302"/>
+      <c r="I45" s="340"/>
+      <c r="J45" s="301"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="100"/>
@@ -14501,87 +14489,87 @@
       <c r="G46" s="46"/>
       <c r="H46" s="126"/>
       <c r="I46" s="126"/>
-      <c r="J46" s="342"/>
+      <c r="J46" s="341"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="109"/>
-      <c r="C47" s="343"/>
-      <c r="D47" s="343"/>
+      <c r="C47" s="342"/>
+      <c r="D47" s="342"/>
       <c r="E47" s="110"/>
-      <c r="F47" s="344"/>
-      <c r="G47" s="344"/>
-      <c r="H47" s="345"/>
-      <c r="I47" s="344"/>
+      <c r="F47" s="343"/>
+      <c r="G47" s="343"/>
+      <c r="H47" s="344"/>
+      <c r="I47" s="343"/>
       <c r="J47" s="153"/>
     </row>
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="94"/>
-      <c r="C48" s="346" t="s">
+      <c r="C48" s="345" t="s">
         <v>188</v>
       </c>
-      <c r="D48" s="346"/>
-      <c r="E48" s="346"/>
-      <c r="F48" s="346"/>
-      <c r="G48" s="346"/>
-      <c r="H48" s="346"/>
-      <c r="I48" s="346"/>
-      <c r="J48" s="346"/>
+      <c r="D48" s="345"/>
+      <c r="E48" s="345"/>
+      <c r="F48" s="345"/>
+      <c r="G48" s="345"/>
+      <c r="H48" s="345"/>
+      <c r="I48" s="345"/>
+      <c r="J48" s="345"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="100"/>
-      <c r="C49" s="346"/>
-      <c r="D49" s="346"/>
-      <c r="E49" s="346"/>
-      <c r="F49" s="346"/>
-      <c r="G49" s="346"/>
-      <c r="H49" s="346"/>
-      <c r="I49" s="346"/>
-      <c r="J49" s="346"/>
+      <c r="C49" s="345"/>
+      <c r="D49" s="345"/>
+      <c r="E49" s="345"/>
+      <c r="F49" s="345"/>
+      <c r="G49" s="345"/>
+      <c r="H49" s="345"/>
+      <c r="I49" s="345"/>
+      <c r="J49" s="345"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="100"/>
-      <c r="C50" s="346"/>
-      <c r="D50" s="346"/>
-      <c r="E50" s="346"/>
-      <c r="F50" s="346"/>
-      <c r="G50" s="346"/>
-      <c r="H50" s="346"/>
-      <c r="I50" s="346"/>
-      <c r="J50" s="346"/>
+      <c r="C50" s="345"/>
+      <c r="D50" s="345"/>
+      <c r="E50" s="345"/>
+      <c r="F50" s="345"/>
+      <c r="G50" s="345"/>
+      <c r="H50" s="345"/>
+      <c r="I50" s="345"/>
+      <c r="J50" s="345"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="100"/>
-      <c r="C51" s="346"/>
-      <c r="D51" s="346"/>
-      <c r="E51" s="346"/>
-      <c r="F51" s="346"/>
-      <c r="G51" s="346"/>
-      <c r="H51" s="346"/>
-      <c r="I51" s="346"/>
-      <c r="J51" s="346"/>
+      <c r="C51" s="345"/>
+      <c r="D51" s="345"/>
+      <c r="E51" s="345"/>
+      <c r="F51" s="345"/>
+      <c r="G51" s="345"/>
+      <c r="H51" s="345"/>
+      <c r="I51" s="345"/>
+      <c r="J51" s="345"/>
     </row>
     <row r="52" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="100"/>
-      <c r="C52" s="346"/>
-      <c r="D52" s="346"/>
-      <c r="E52" s="346"/>
-      <c r="F52" s="346"/>
-      <c r="G52" s="346"/>
-      <c r="H52" s="346"/>
-      <c r="I52" s="346"/>
-      <c r="J52" s="346"/>
+      <c r="C52" s="345"/>
+      <c r="D52" s="345"/>
+      <c r="E52" s="345"/>
+      <c r="F52" s="345"/>
+      <c r="G52" s="345"/>
+      <c r="H52" s="345"/>
+      <c r="I52" s="345"/>
+      <c r="J52" s="345"/>
     </row>
     <row r="53" customFormat="false" ht="33.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="151"/>
-      <c r="C53" s="346"/>
-      <c r="D53" s="346"/>
-      <c r="E53" s="346"/>
-      <c r="F53" s="346"/>
-      <c r="G53" s="346"/>
-      <c r="H53" s="346"/>
-      <c r="I53" s="346"/>
-      <c r="J53" s="346"/>
-      <c r="K53" s="347"/>
+      <c r="C53" s="345"/>
+      <c r="D53" s="345"/>
+      <c r="E53" s="345"/>
+      <c r="F53" s="345"/>
+      <c r="G53" s="345"/>
+      <c r="H53" s="345"/>
+      <c r="I53" s="345"/>
+      <c r="J53" s="345"/>
+      <c r="K53" s="346"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -15083,14 +15071,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="2" s="348" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="349" t="s">
+    <row r="2" s="347" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="348" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="349"/>
-      <c r="D2" s="349"/>
-      <c r="E2" s="349"/>
-      <c r="F2" s="349"/>
+      <c r="C2" s="348"/>
+      <c r="D2" s="348"/>
+      <c r="E2" s="348"/>
+      <c r="F2" s="348"/>
       <c r="ALG2" s="0"/>
       <c r="ALH2" s="0"/>
       <c r="ALI2" s="0"/>
@@ -15123,119 +15111,119 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="350" t="s">
+      <c r="B3" s="349" t="s">
         <v>190</v>
       </c>
-      <c r="C3" s="350"/>
-      <c r="D3" s="350"/>
-      <c r="E3" s="350"/>
-      <c r="F3" s="350"/>
+      <c r="C3" s="349"/>
+      <c r="D3" s="349"/>
+      <c r="E3" s="349"/>
+      <c r="F3" s="349"/>
     </row>
     <row r="4" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="351" t="s">
+      <c r="B4" s="350" t="s">
         <v>191</v>
       </c>
       <c r="C4" s="97"/>
-      <c r="D4" s="352"/>
-      <c r="E4" s="352"/>
-      <c r="F4" s="353"/>
+      <c r="D4" s="351"/>
+      <c r="E4" s="351"/>
+      <c r="F4" s="352"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="323"/>
-      <c r="C5" s="323"/>
-      <c r="D5" s="323"/>
-      <c r="E5" s="323"/>
-      <c r="F5" s="323"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="322"/>
+      <c r="E5" s="322"/>
+      <c r="F5" s="322"/>
       <c r="G5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="323"/>
-      <c r="C6" s="323"/>
-      <c r="D6" s="323"/>
-      <c r="E6" s="323"/>
-      <c r="F6" s="323"/>
+      <c r="B6" s="322"/>
+      <c r="C6" s="322"/>
+      <c r="D6" s="322"/>
+      <c r="E6" s="322"/>
+      <c r="F6" s="322"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="323"/>
-      <c r="C7" s="323"/>
-      <c r="D7" s="323"/>
-      <c r="E7" s="323"/>
-      <c r="F7" s="323"/>
+      <c r="B7" s="322"/>
+      <c r="C7" s="322"/>
+      <c r="D7" s="322"/>
+      <c r="E7" s="322"/>
+      <c r="F7" s="322"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="323"/>
-      <c r="C8" s="323"/>
-      <c r="D8" s="323"/>
-      <c r="E8" s="323"/>
-      <c r="F8" s="323"/>
+      <c r="B8" s="322"/>
+      <c r="C8" s="322"/>
+      <c r="D8" s="322"/>
+      <c r="E8" s="322"/>
+      <c r="F8" s="322"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="323"/>
-      <c r="C9" s="323"/>
-      <c r="D9" s="323"/>
-      <c r="E9" s="323"/>
-      <c r="F9" s="323"/>
+      <c r="B9" s="322"/>
+      <c r="C9" s="322"/>
+      <c r="D9" s="322"/>
+      <c r="E9" s="322"/>
+      <c r="F9" s="322"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="328"/>
-      <c r="C10" s="328"/>
-      <c r="D10" s="328"/>
-      <c r="E10" s="328"/>
-      <c r="F10" s="328"/>
+      <c r="B10" s="327"/>
+      <c r="C10" s="327"/>
+      <c r="D10" s="327"/>
+      <c r="E10" s="327"/>
+      <c r="F10" s="327"/>
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="354" t="s">
+      <c r="B11" s="353" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="354"/>
-      <c r="D11" s="354"/>
-      <c r="E11" s="354"/>
-      <c r="F11" s="354"/>
+      <c r="C11" s="353"/>
+      <c r="D11" s="353"/>
+      <c r="E11" s="353"/>
+      <c r="F11" s="353"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="355" t="n">
+      <c r="B12" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="356"/>
-      <c r="D12" s="356"/>
-      <c r="E12" s="356"/>
-      <c r="F12" s="356"/>
+      <c r="C12" s="355"/>
+      <c r="D12" s="355"/>
+      <c r="E12" s="355"/>
+      <c r="F12" s="355"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="355" t="n">
+      <c r="B13" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="356"/>
-      <c r="D13" s="356"/>
-      <c r="E13" s="356"/>
-      <c r="F13" s="356"/>
+      <c r="C13" s="355"/>
+      <c r="D13" s="355"/>
+      <c r="E13" s="355"/>
+      <c r="F13" s="355"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="355" t="n">
+      <c r="B14" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="356"/>
-      <c r="D14" s="356"/>
-      <c r="E14" s="356"/>
-      <c r="F14" s="356"/>
+      <c r="C14" s="355"/>
+      <c r="D14" s="355"/>
+      <c r="E14" s="355"/>
+      <c r="F14" s="355"/>
     </row>
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="357"/>
-      <c r="C15" s="358" t="s">
+      <c r="B15" s="356"/>
+      <c r="C15" s="357" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="358" t="s">
+      <c r="D15" s="357" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="358" t="s">
+      <c r="E15" s="357" t="s">
         <v>195</v>
       </c>
-      <c r="F15" s="359" t="s">
+      <c r="F15" s="358" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="360"/>
+      <c r="B16" s="359"/>
       <c r="C16" s="115" t="s">
         <v>30</v>
       </c>
@@ -15250,138 +15238,138 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="355" t="n">
+      <c r="B17" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="361"/>
-      <c r="D17" s="361"/>
-      <c r="E17" s="361"/>
-      <c r="F17" s="361"/>
+      <c r="C17" s="360"/>
+      <c r="D17" s="360"/>
+      <c r="E17" s="360"/>
+      <c r="F17" s="360"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="355" t="n">
+      <c r="B18" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="361"/>
-      <c r="D18" s="361"/>
-      <c r="E18" s="361"/>
-      <c r="F18" s="361"/>
+      <c r="C18" s="360"/>
+      <c r="D18" s="360"/>
+      <c r="E18" s="360"/>
+      <c r="F18" s="360"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="355" t="n">
+      <c r="B19" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="361"/>
-      <c r="D19" s="361"/>
-      <c r="E19" s="361"/>
-      <c r="F19" s="361"/>
+      <c r="C19" s="360"/>
+      <c r="D19" s="360"/>
+      <c r="E19" s="360"/>
+      <c r="F19" s="360"/>
     </row>
     <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="362" t="s">
+      <c r="B20" s="361" t="s">
         <v>197</v>
       </c>
       <c r="C20" s="97"/>
-      <c r="D20" s="352"/>
-      <c r="E20" s="352"/>
-      <c r="F20" s="363"/>
+      <c r="D20" s="351"/>
+      <c r="E20" s="351"/>
+      <c r="F20" s="362"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="323"/>
-      <c r="C21" s="323"/>
-      <c r="D21" s="323"/>
-      <c r="E21" s="323"/>
-      <c r="F21" s="323"/>
+      <c r="B21" s="322"/>
+      <c r="C21" s="322"/>
+      <c r="D21" s="322"/>
+      <c r="E21" s="322"/>
+      <c r="F21" s="322"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="323"/>
-      <c r="C22" s="323"/>
-      <c r="D22" s="323"/>
-      <c r="E22" s="323"/>
-      <c r="F22" s="323"/>
+      <c r="B22" s="322"/>
+      <c r="C22" s="322"/>
+      <c r="D22" s="322"/>
+      <c r="E22" s="322"/>
+      <c r="F22" s="322"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="323"/>
-      <c r="C23" s="323"/>
-      <c r="D23" s="323"/>
-      <c r="E23" s="323"/>
-      <c r="F23" s="323"/>
+      <c r="B23" s="322"/>
+      <c r="C23" s="322"/>
+      <c r="D23" s="322"/>
+      <c r="E23" s="322"/>
+      <c r="F23" s="322"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="323"/>
-      <c r="C24" s="323"/>
-      <c r="D24" s="323"/>
-      <c r="E24" s="323"/>
-      <c r="F24" s="323"/>
+      <c r="B24" s="322"/>
+      <c r="C24" s="322"/>
+      <c r="D24" s="322"/>
+      <c r="E24" s="322"/>
+      <c r="F24" s="322"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="323"/>
-      <c r="C25" s="323"/>
-      <c r="D25" s="323"/>
-      <c r="E25" s="323"/>
-      <c r="F25" s="323"/>
+      <c r="B25" s="322"/>
+      <c r="C25" s="322"/>
+      <c r="D25" s="322"/>
+      <c r="E25" s="322"/>
+      <c r="F25" s="322"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="328" t="s">
+      <c r="B26" s="327" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="328"/>
-      <c r="D26" s="328"/>
-      <c r="E26" s="328"/>
-      <c r="F26" s="328"/>
+      <c r="C26" s="327"/>
+      <c r="D26" s="327"/>
+      <c r="E26" s="327"/>
+      <c r="F26" s="327"/>
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="354" t="s">
+      <c r="B27" s="353" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="354"/>
-      <c r="D27" s="354"/>
-      <c r="E27" s="354"/>
-      <c r="F27" s="354"/>
+      <c r="C27" s="353"/>
+      <c r="D27" s="353"/>
+      <c r="E27" s="353"/>
+      <c r="F27" s="353"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="355" t="n">
+      <c r="B28" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C28" s="356"/>
-      <c r="D28" s="356"/>
-      <c r="E28" s="356"/>
-      <c r="F28" s="356"/>
+      <c r="C28" s="355"/>
+      <c r="D28" s="355"/>
+      <c r="E28" s="355"/>
+      <c r="F28" s="355"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="355" t="n">
+      <c r="B29" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C29" s="356"/>
-      <c r="D29" s="356"/>
-      <c r="E29" s="356"/>
-      <c r="F29" s="356"/>
+      <c r="C29" s="355"/>
+      <c r="D29" s="355"/>
+      <c r="E29" s="355"/>
+      <c r="F29" s="355"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="355" t="n">
+      <c r="B30" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C30" s="356"/>
-      <c r="D30" s="356"/>
-      <c r="E30" s="356"/>
-      <c r="F30" s="356"/>
+      <c r="C30" s="355"/>
+      <c r="D30" s="355"/>
+      <c r="E30" s="355"/>
+      <c r="F30" s="355"/>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="364"/>
-      <c r="C31" s="358" t="s">
+      <c r="B31" s="363"/>
+      <c r="C31" s="357" t="s">
         <v>193</v>
       </c>
-      <c r="D31" s="358" t="s">
+      <c r="D31" s="357" t="s">
         <v>198</v>
       </c>
-      <c r="E31" s="358" t="s">
+      <c r="E31" s="357" t="s">
         <v>199</v>
       </c>
-      <c r="F31" s="359" t="s">
+      <c r="F31" s="358" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="364"/>
+      <c r="B32" s="363"/>
       <c r="C32" s="115" t="s">
         <v>30</v>
       </c>
@@ -15396,136 +15384,136 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="355" t="n">
+      <c r="B33" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="361"/>
-      <c r="D33" s="361"/>
-      <c r="E33" s="361"/>
-      <c r="F33" s="361"/>
+      <c r="C33" s="360"/>
+      <c r="D33" s="360"/>
+      <c r="E33" s="360"/>
+      <c r="F33" s="360"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="355" t="n">
+      <c r="B34" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C34" s="361"/>
-      <c r="D34" s="361"/>
-      <c r="E34" s="361"/>
-      <c r="F34" s="361"/>
+      <c r="C34" s="360"/>
+      <c r="D34" s="360"/>
+      <c r="E34" s="360"/>
+      <c r="F34" s="360"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="355" t="n">
+      <c r="B35" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C35" s="361"/>
-      <c r="D35" s="361"/>
-      <c r="E35" s="361"/>
-      <c r="F35" s="361"/>
+      <c r="C35" s="360"/>
+      <c r="D35" s="360"/>
+      <c r="E35" s="360"/>
+      <c r="F35" s="360"/>
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="362" t="s">
+      <c r="B36" s="361" t="s">
         <v>200</v>
       </c>
-      <c r="C36" s="365"/>
+      <c r="C36" s="364"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
-      <c r="F36" s="363"/>
+      <c r="F36" s="362"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="323"/>
-      <c r="C37" s="323"/>
-      <c r="D37" s="323"/>
-      <c r="E37" s="323"/>
-      <c r="F37" s="323"/>
+      <c r="B37" s="322"/>
+      <c r="C37" s="322"/>
+      <c r="D37" s="322"/>
+      <c r="E37" s="322"/>
+      <c r="F37" s="322"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="323"/>
-      <c r="C38" s="323"/>
-      <c r="D38" s="323"/>
-      <c r="E38" s="323"/>
-      <c r="F38" s="323"/>
+      <c r="B38" s="322"/>
+      <c r="C38" s="322"/>
+      <c r="D38" s="322"/>
+      <c r="E38" s="322"/>
+      <c r="F38" s="322"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="323"/>
-      <c r="C39" s="323"/>
-      <c r="D39" s="323"/>
-      <c r="E39" s="323"/>
-      <c r="F39" s="323"/>
+      <c r="B39" s="322"/>
+      <c r="C39" s="322"/>
+      <c r="D39" s="322"/>
+      <c r="E39" s="322"/>
+      <c r="F39" s="322"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="323"/>
-      <c r="C40" s="323"/>
-      <c r="D40" s="323"/>
-      <c r="E40" s="323"/>
-      <c r="F40" s="323"/>
+      <c r="B40" s="322"/>
+      <c r="C40" s="322"/>
+      <c r="D40" s="322"/>
+      <c r="E40" s="322"/>
+      <c r="F40" s="322"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="323"/>
-      <c r="C41" s="323"/>
-      <c r="D41" s="323"/>
-      <c r="E41" s="323"/>
-      <c r="F41" s="323"/>
+      <c r="B41" s="322"/>
+      <c r="C41" s="322"/>
+      <c r="D41" s="322"/>
+      <c r="E41" s="322"/>
+      <c r="F41" s="322"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="328"/>
-      <c r="C42" s="328"/>
-      <c r="D42" s="328"/>
-      <c r="E42" s="328"/>
-      <c r="F42" s="328"/>
+      <c r="B42" s="327"/>
+      <c r="C42" s="327"/>
+      <c r="D42" s="327"/>
+      <c r="E42" s="327"/>
+      <c r="F42" s="327"/>
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="354" t="s">
+      <c r="B43" s="353" t="s">
         <v>192</v>
       </c>
-      <c r="C43" s="354"/>
-      <c r="D43" s="354"/>
-      <c r="E43" s="354"/>
-      <c r="F43" s="354"/>
+      <c r="C43" s="353"/>
+      <c r="D43" s="353"/>
+      <c r="E43" s="353"/>
+      <c r="F43" s="353"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="355" t="n">
+      <c r="B44" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="356"/>
-      <c r="D44" s="356"/>
-      <c r="E44" s="356"/>
-      <c r="F44" s="356"/>
+      <c r="C44" s="355"/>
+      <c r="D44" s="355"/>
+      <c r="E44" s="355"/>
+      <c r="F44" s="355"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="355" t="n">
+      <c r="B45" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C45" s="356"/>
-      <c r="D45" s="356"/>
-      <c r="E45" s="356"/>
-      <c r="F45" s="356"/>
+      <c r="C45" s="355"/>
+      <c r="D45" s="355"/>
+      <c r="E45" s="355"/>
+      <c r="F45" s="355"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="355" t="n">
+      <c r="B46" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C46" s="356"/>
-      <c r="D46" s="356"/>
-      <c r="E46" s="356"/>
-      <c r="F46" s="356"/>
+      <c r="C46" s="355"/>
+      <c r="D46" s="355"/>
+      <c r="E46" s="355"/>
+      <c r="F46" s="355"/>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="364"/>
-      <c r="C47" s="358" t="s">
+      <c r="B47" s="363"/>
+      <c r="C47" s="357" t="s">
         <v>201</v>
       </c>
-      <c r="D47" s="358" t="s">
+      <c r="D47" s="357" t="s">
         <v>198</v>
       </c>
-      <c r="E47" s="358" t="s">
+      <c r="E47" s="357" t="s">
         <v>199</v>
       </c>
-      <c r="F47" s="359" t="s">
+      <c r="F47" s="358" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="364"/>
+      <c r="B48" s="363"/>
       <c r="C48" s="115" t="s">
         <v>30</v>
       </c>
@@ -15540,31 +15528,31 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="355" t="n">
+      <c r="B49" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C49" s="361"/>
-      <c r="D49" s="361"/>
-      <c r="E49" s="361"/>
-      <c r="F49" s="361"/>
+      <c r="C49" s="360"/>
+      <c r="D49" s="360"/>
+      <c r="E49" s="360"/>
+      <c r="F49" s="360"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="355" t="n">
+      <c r="B50" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C50" s="361"/>
-      <c r="D50" s="361"/>
-      <c r="E50" s="361"/>
-      <c r="F50" s="361"/>
+      <c r="C50" s="360"/>
+      <c r="D50" s="360"/>
+      <c r="E50" s="360"/>
+      <c r="F50" s="360"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="355" t="n">
+      <c r="B51" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C51" s="361"/>
-      <c r="D51" s="361"/>
-      <c r="E51" s="361"/>
-      <c r="F51" s="361"/>
+      <c r="C51" s="360"/>
+      <c r="D51" s="360"/>
+      <c r="E51" s="360"/>
+      <c r="F51" s="360"/>
     </row>
     <row r="52" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -15784,118 +15772,118 @@
   <sheetData>
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="351" t="s">
+      <c r="B2" s="350" t="s">
         <v>202</v>
       </c>
       <c r="C2" s="97"/>
-      <c r="D2" s="352"/>
-      <c r="E2" s="352"/>
-      <c r="F2" s="353"/>
+      <c r="D2" s="351"/>
+      <c r="E2" s="351"/>
+      <c r="F2" s="352"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="323"/>
-      <c r="C3" s="323"/>
-      <c r="D3" s="323"/>
-      <c r="E3" s="323"/>
-      <c r="F3" s="323"/>
+      <c r="B3" s="322"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="323"/>
-      <c r="C4" s="323"/>
-      <c r="D4" s="323"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="323"/>
+      <c r="B4" s="322"/>
+      <c r="C4" s="322"/>
+      <c r="D4" s="322"/>
+      <c r="E4" s="322"/>
+      <c r="F4" s="322"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="323"/>
-      <c r="C5" s="323"/>
-      <c r="D5" s="323"/>
-      <c r="E5" s="323"/>
-      <c r="F5" s="323"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="322"/>
+      <c r="E5" s="322"/>
+      <c r="F5" s="322"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="323"/>
-      <c r="C6" s="323"/>
-      <c r="D6" s="323"/>
-      <c r="E6" s="323"/>
-      <c r="F6" s="323"/>
+      <c r="B6" s="322"/>
+      <c r="C6" s="322"/>
+      <c r="D6" s="322"/>
+      <c r="E6" s="322"/>
+      <c r="F6" s="322"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="323"/>
-      <c r="C7" s="323"/>
-      <c r="D7" s="323"/>
-      <c r="E7" s="323"/>
-      <c r="F7" s="323"/>
+      <c r="B7" s="322"/>
+      <c r="C7" s="322"/>
+      <c r="D7" s="322"/>
+      <c r="E7" s="322"/>
+      <c r="F7" s="322"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="323"/>
-      <c r="C8" s="323"/>
-      <c r="D8" s="323"/>
-      <c r="E8" s="323"/>
-      <c r="F8" s="323"/>
+      <c r="B8" s="322"/>
+      <c r="C8" s="322"/>
+      <c r="D8" s="322"/>
+      <c r="E8" s="322"/>
+      <c r="F8" s="322"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="328"/>
-      <c r="C9" s="328"/>
-      <c r="D9" s="328"/>
-      <c r="E9" s="328"/>
-      <c r="F9" s="328"/>
+      <c r="B9" s="327"/>
+      <c r="C9" s="327"/>
+      <c r="D9" s="327"/>
+      <c r="E9" s="327"/>
+      <c r="F9" s="327"/>
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="366" t="s">
+      <c r="B10" s="365" t="s">
         <v>192</v>
       </c>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="365"/>
+      <c r="D10" s="365"/>
+      <c r="E10" s="365"/>
+      <c r="F10" s="365"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="355" t="n">
+      <c r="B11" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="367"/>
-      <c r="D11" s="367"/>
-      <c r="E11" s="367"/>
-      <c r="F11" s="367"/>
+      <c r="C11" s="366"/>
+      <c r="D11" s="366"/>
+      <c r="E11" s="366"/>
+      <c r="F11" s="366"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="355" t="n">
+      <c r="B12" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="367"/>
-      <c r="D12" s="367"/>
-      <c r="E12" s="367"/>
-      <c r="F12" s="367"/>
+      <c r="C12" s="366"/>
+      <c r="D12" s="366"/>
+      <c r="E12" s="366"/>
+      <c r="F12" s="366"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="355" t="n">
+      <c r="B13" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="367"/>
-      <c r="D13" s="367"/>
-      <c r="E13" s="367"/>
-      <c r="F13" s="367"/>
+      <c r="C13" s="366"/>
+      <c r="D13" s="366"/>
+      <c r="E13" s="366"/>
+      <c r="F13" s="366"/>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="364"/>
-      <c r="C14" s="358" t="s">
+      <c r="B14" s="363"/>
+      <c r="C14" s="357" t="s">
         <v>201</v>
       </c>
-      <c r="D14" s="358" t="s">
+      <c r="D14" s="357" t="s">
         <v>198</v>
       </c>
-      <c r="E14" s="358" t="s">
+      <c r="E14" s="357" t="s">
         <v>199</v>
       </c>
-      <c r="F14" s="359" t="s">
+      <c r="F14" s="358" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="364"/>
+      <c r="B15" s="363"/>
       <c r="C15" s="115" t="s">
         <v>30</v>
       </c>
@@ -15910,143 +15898,143 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="355" t="n">
+      <c r="B16" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="361"/>
-      <c r="D16" s="361"/>
-      <c r="E16" s="361"/>
-      <c r="F16" s="361"/>
+      <c r="C16" s="360"/>
+      <c r="D16" s="360"/>
+      <c r="E16" s="360"/>
+      <c r="F16" s="360"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="355" t="n">
+      <c r="B17" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="361"/>
-      <c r="D17" s="361"/>
-      <c r="E17" s="361"/>
-      <c r="F17" s="361"/>
+      <c r="C17" s="360"/>
+      <c r="D17" s="360"/>
+      <c r="E17" s="360"/>
+      <c r="F17" s="360"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="355" t="n">
+      <c r="B18" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="361"/>
-      <c r="D18" s="361"/>
-      <c r="E18" s="361"/>
-      <c r="F18" s="361"/>
+      <c r="C18" s="360"/>
+      <c r="D18" s="360"/>
+      <c r="E18" s="360"/>
+      <c r="F18" s="360"/>
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="362" t="s">
+      <c r="B19" s="361" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="365"/>
+      <c r="C19" s="364"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="363"/>
+      <c r="F19" s="362"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="323"/>
-      <c r="C20" s="323"/>
-      <c r="D20" s="323"/>
-      <c r="E20" s="323"/>
-      <c r="F20" s="323"/>
+      <c r="B20" s="322"/>
+      <c r="C20" s="322"/>
+      <c r="D20" s="322"/>
+      <c r="E20" s="322"/>
+      <c r="F20" s="322"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="323"/>
-      <c r="C21" s="323"/>
-      <c r="D21" s="323"/>
-      <c r="E21" s="323"/>
-      <c r="F21" s="323"/>
+      <c r="B21" s="322"/>
+      <c r="C21" s="322"/>
+      <c r="D21" s="322"/>
+      <c r="E21" s="322"/>
+      <c r="F21" s="322"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="323"/>
-      <c r="C22" s="323"/>
-      <c r="D22" s="323"/>
-      <c r="E22" s="323"/>
-      <c r="F22" s="323"/>
+      <c r="B22" s="322"/>
+      <c r="C22" s="322"/>
+      <c r="D22" s="322"/>
+      <c r="E22" s="322"/>
+      <c r="F22" s="322"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="323"/>
-      <c r="C23" s="323"/>
-      <c r="D23" s="323"/>
-      <c r="E23" s="323"/>
-      <c r="F23" s="323"/>
+      <c r="B23" s="322"/>
+      <c r="C23" s="322"/>
+      <c r="D23" s="322"/>
+      <c r="E23" s="322"/>
+      <c r="F23" s="322"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="323"/>
-      <c r="C24" s="323"/>
-      <c r="D24" s="323"/>
-      <c r="E24" s="323"/>
-      <c r="F24" s="323"/>
+      <c r="B24" s="322"/>
+      <c r="C24" s="322"/>
+      <c r="D24" s="322"/>
+      <c r="E24" s="322"/>
+      <c r="F24" s="322"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="323"/>
-      <c r="C25" s="323"/>
-      <c r="D25" s="323"/>
-      <c r="E25" s="323"/>
-      <c r="F25" s="323"/>
+      <c r="B25" s="322"/>
+      <c r="C25" s="322"/>
+      <c r="D25" s="322"/>
+      <c r="E25" s="322"/>
+      <c r="F25" s="322"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="323"/>
-      <c r="C26" s="323"/>
-      <c r="D26" s="323"/>
-      <c r="E26" s="323"/>
-      <c r="F26" s="323"/>
+      <c r="B26" s="322"/>
+      <c r="C26" s="322"/>
+      <c r="D26" s="322"/>
+      <c r="E26" s="322"/>
+      <c r="F26" s="322"/>
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="366" t="s">
+      <c r="B27" s="365" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="366"/>
-      <c r="D27" s="366"/>
-      <c r="E27" s="366"/>
-      <c r="F27" s="366"/>
+      <c r="C27" s="365"/>
+      <c r="D27" s="365"/>
+      <c r="E27" s="365"/>
+      <c r="F27" s="365"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="355" t="n">
+      <c r="B28" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C28" s="367"/>
-      <c r="D28" s="367"/>
-      <c r="E28" s="367"/>
-      <c r="F28" s="367"/>
+      <c r="C28" s="366"/>
+      <c r="D28" s="366"/>
+      <c r="E28" s="366"/>
+      <c r="F28" s="366"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="355" t="n">
+      <c r="B29" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C29" s="367"/>
-      <c r="D29" s="367"/>
-      <c r="E29" s="367"/>
-      <c r="F29" s="367"/>
+      <c r="C29" s="366"/>
+      <c r="D29" s="366"/>
+      <c r="E29" s="366"/>
+      <c r="F29" s="366"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="355" t="n">
+      <c r="B30" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C30" s="367"/>
-      <c r="D30" s="367"/>
-      <c r="E30" s="367"/>
-      <c r="F30" s="367"/>
+      <c r="C30" s="366"/>
+      <c r="D30" s="366"/>
+      <c r="E30" s="366"/>
+      <c r="F30" s="366"/>
     </row>
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="364"/>
-      <c r="C31" s="358" t="s">
+      <c r="B31" s="363"/>
+      <c r="C31" s="357" t="s">
         <v>201</v>
       </c>
-      <c r="D31" s="358" t="s">
+      <c r="D31" s="357" t="s">
         <v>198</v>
       </c>
-      <c r="E31" s="358" t="s">
+      <c r="E31" s="357" t="s">
         <v>199</v>
       </c>
-      <c r="F31" s="359" t="s">
+      <c r="F31" s="358" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="364"/>
+      <c r="B32" s="363"/>
       <c r="C32" s="115" t="s">
         <v>30</v>
       </c>
@@ -16061,198 +16049,198 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="355" t="n">
+      <c r="B33" s="354" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="361"/>
-      <c r="D33" s="361"/>
-      <c r="E33" s="361"/>
-      <c r="F33" s="361"/>
+      <c r="C33" s="360"/>
+      <c r="D33" s="360"/>
+      <c r="E33" s="360"/>
+      <c r="F33" s="360"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="355" t="n">
+      <c r="B34" s="354" t="n">
         <v>2</v>
       </c>
-      <c r="C34" s="361"/>
-      <c r="D34" s="361"/>
-      <c r="E34" s="361"/>
-      <c r="F34" s="361"/>
+      <c r="C34" s="360"/>
+      <c r="D34" s="360"/>
+      <c r="E34" s="360"/>
+      <c r="F34" s="360"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="355" t="n">
+      <c r="B35" s="354" t="n">
         <v>3</v>
       </c>
-      <c r="C35" s="361"/>
-      <c r="D35" s="361"/>
-      <c r="E35" s="361"/>
-      <c r="F35" s="361"/>
+      <c r="C35" s="360"/>
+      <c r="D35" s="360"/>
+      <c r="E35" s="360"/>
+      <c r="F35" s="360"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="368" t="s">
+      <c r="B36" s="367" t="s">
         <v>204</v>
       </c>
-      <c r="C36" s="368"/>
-      <c r="D36" s="368"/>
-      <c r="E36" s="368"/>
-      <c r="F36" s="368"/>
+      <c r="C36" s="367"/>
+      <c r="D36" s="367"/>
+      <c r="E36" s="367"/>
+      <c r="F36" s="367"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="323"/>
-      <c r="C37" s="323"/>
-      <c r="D37" s="323"/>
-      <c r="E37" s="323"/>
-      <c r="F37" s="323"/>
+      <c r="B37" s="322"/>
+      <c r="C37" s="322"/>
+      <c r="D37" s="322"/>
+      <c r="E37" s="322"/>
+      <c r="F37" s="322"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="323"/>
-      <c r="C38" s="323"/>
-      <c r="D38" s="323"/>
-      <c r="E38" s="323"/>
-      <c r="F38" s="323"/>
+      <c r="B38" s="322"/>
+      <c r="C38" s="322"/>
+      <c r="D38" s="322"/>
+      <c r="E38" s="322"/>
+      <c r="F38" s="322"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="323"/>
-      <c r="C39" s="323"/>
-      <c r="D39" s="323"/>
-      <c r="E39" s="323"/>
-      <c r="F39" s="323"/>
+      <c r="B39" s="322"/>
+      <c r="C39" s="322"/>
+      <c r="D39" s="322"/>
+      <c r="E39" s="322"/>
+      <c r="F39" s="322"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="323"/>
-      <c r="C40" s="323"/>
-      <c r="D40" s="323"/>
-      <c r="E40" s="323"/>
-      <c r="F40" s="323"/>
+      <c r="B40" s="322"/>
+      <c r="C40" s="322"/>
+      <c r="D40" s="322"/>
+      <c r="E40" s="322"/>
+      <c r="F40" s="322"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="323"/>
-      <c r="C41" s="323"/>
-      <c r="D41" s="323"/>
-      <c r="E41" s="323"/>
-      <c r="F41" s="323"/>
+      <c r="B41" s="322"/>
+      <c r="C41" s="322"/>
+      <c r="D41" s="322"/>
+      <c r="E41" s="322"/>
+      <c r="F41" s="322"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="323"/>
-      <c r="C42" s="323"/>
-      <c r="D42" s="323"/>
-      <c r="E42" s="323"/>
-      <c r="F42" s="323"/>
+      <c r="B42" s="322"/>
+      <c r="C42" s="322"/>
+      <c r="D42" s="322"/>
+      <c r="E42" s="322"/>
+      <c r="F42" s="322"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="369"/>
-      <c r="C43" s="369"/>
-      <c r="D43" s="369"/>
-      <c r="E43" s="369"/>
-      <c r="F43" s="369"/>
+      <c r="B43" s="368"/>
+      <c r="C43" s="368"/>
+      <c r="D43" s="368"/>
+      <c r="E43" s="368"/>
+      <c r="F43" s="368"/>
     </row>
     <row r="44" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="323"/>
-      <c r="C44" s="323"/>
-      <c r="D44" s="323"/>
-      <c r="E44" s="323"/>
-      <c r="F44" s="323"/>
+      <c r="B44" s="322"/>
+      <c r="C44" s="322"/>
+      <c r="D44" s="322"/>
+      <c r="E44" s="322"/>
+      <c r="F44" s="322"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="323"/>
-      <c r="C45" s="323"/>
-      <c r="D45" s="323"/>
-      <c r="E45" s="323"/>
-      <c r="F45" s="323"/>
+      <c r="B45" s="322"/>
+      <c r="C45" s="322"/>
+      <c r="D45" s="322"/>
+      <c r="E45" s="322"/>
+      <c r="F45" s="322"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="323"/>
-      <c r="C46" s="323"/>
-      <c r="D46" s="323"/>
-      <c r="E46" s="323"/>
-      <c r="F46" s="323"/>
+      <c r="B46" s="322"/>
+      <c r="C46" s="322"/>
+      <c r="D46" s="322"/>
+      <c r="E46" s="322"/>
+      <c r="F46" s="322"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="323"/>
-      <c r="C47" s="323"/>
-      <c r="D47" s="323"/>
-      <c r="E47" s="323"/>
-      <c r="F47" s="323"/>
+      <c r="B47" s="322"/>
+      <c r="C47" s="322"/>
+      <c r="D47" s="322"/>
+      <c r="E47" s="322"/>
+      <c r="F47" s="322"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="323"/>
-      <c r="C48" s="323"/>
-      <c r="D48" s="323"/>
-      <c r="E48" s="323"/>
-      <c r="F48" s="323"/>
+      <c r="B48" s="322"/>
+      <c r="C48" s="322"/>
+      <c r="D48" s="322"/>
+      <c r="E48" s="322"/>
+      <c r="F48" s="322"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="323"/>
-      <c r="C49" s="323"/>
-      <c r="D49" s="323"/>
-      <c r="E49" s="323"/>
-      <c r="F49" s="323"/>
+      <c r="B49" s="322"/>
+      <c r="C49" s="322"/>
+      <c r="D49" s="322"/>
+      <c r="E49" s="322"/>
+      <c r="F49" s="322"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="323"/>
-      <c r="C50" s="323"/>
-      <c r="D50" s="323"/>
-      <c r="E50" s="323"/>
-      <c r="F50" s="323"/>
+      <c r="B50" s="322"/>
+      <c r="C50" s="322"/>
+      <c r="D50" s="322"/>
+      <c r="E50" s="322"/>
+      <c r="F50" s="322"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="323"/>
-      <c r="C51" s="323"/>
-      <c r="D51" s="323"/>
-      <c r="E51" s="323"/>
-      <c r="F51" s="323"/>
+      <c r="B51" s="322"/>
+      <c r="C51" s="322"/>
+      <c r="D51" s="322"/>
+      <c r="E51" s="322"/>
+      <c r="F51" s="322"/>
     </row>
     <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="351" t="s">
+      <c r="B52" s="350" t="s">
         <v>205</v>
       </c>
       <c r="C52" s="97"/>
-      <c r="D52" s="352"/>
-      <c r="E52" s="352"/>
-      <c r="F52" s="353"/>
+      <c r="D52" s="351"/>
+      <c r="E52" s="351"/>
+      <c r="F52" s="352"/>
     </row>
     <row r="53" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="157"/>
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="370"/>
+      <c r="F53" s="369"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="317" t="s">
+      <c r="B54" s="316" t="s">
         <v>206</v>
       </c>
-      <c r="C54" s="317"/>
-      <c r="D54" s="317"/>
-      <c r="E54" s="317"/>
-      <c r="F54" s="317"/>
+      <c r="C54" s="316"/>
+      <c r="D54" s="316"/>
+      <c r="E54" s="316"/>
+      <c r="F54" s="316"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="323"/>
-      <c r="C55" s="323"/>
-      <c r="D55" s="323"/>
-      <c r="E55" s="323"/>
-      <c r="F55" s="323"/>
+      <c r="B55" s="322"/>
+      <c r="C55" s="322"/>
+      <c r="D55" s="322"/>
+      <c r="E55" s="322"/>
+      <c r="F55" s="322"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="323"/>
-      <c r="C56" s="323"/>
-      <c r="D56" s="323"/>
-      <c r="E56" s="323"/>
-      <c r="F56" s="323"/>
+      <c r="B56" s="322"/>
+      <c r="C56" s="322"/>
+      <c r="D56" s="322"/>
+      <c r="E56" s="322"/>
+      <c r="F56" s="322"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="323"/>
-      <c r="C57" s="323"/>
-      <c r="D57" s="323"/>
-      <c r="E57" s="323"/>
-      <c r="F57" s="323"/>
+      <c r="B57" s="322"/>
+      <c r="C57" s="322"/>
+      <c r="D57" s="322"/>
+      <c r="E57" s="322"/>
+      <c r="F57" s="322"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="151"/>
       <c r="C58" s="152"/>
       <c r="D58" s="152"/>
       <c r="E58" s="152"/>
-      <c r="F58" s="371"/>
+      <c r="F58" s="370"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -16421,539 +16409,539 @@
   <sheetData>
     <row r="1" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="372" t="s">
+      <c r="B2" s="371" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="372"/>
-      <c r="D2" s="372"/>
-      <c r="E2" s="372"/>
-      <c r="F2" s="372"/>
-      <c r="G2" s="372"/>
-      <c r="H2" s="372"/>
+      <c r="C2" s="371"/>
+      <c r="D2" s="371"/>
+      <c r="E2" s="371"/>
+      <c r="F2" s="371"/>
+      <c r="G2" s="371"/>
+      <c r="H2" s="371"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="323"/>
-      <c r="C3" s="323"/>
-      <c r="D3" s="323"/>
-      <c r="E3" s="323"/>
-      <c r="F3" s="323"/>
-      <c r="G3" s="323"/>
-      <c r="H3" s="323"/>
+      <c r="B3" s="322"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="322"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="323"/>
-      <c r="C4" s="323"/>
-      <c r="D4" s="323"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="323"/>
-      <c r="G4" s="323"/>
-      <c r="H4" s="323"/>
+      <c r="B4" s="322"/>
+      <c r="C4" s="322"/>
+      <c r="D4" s="322"/>
+      <c r="E4" s="322"/>
+      <c r="F4" s="322"/>
+      <c r="G4" s="322"/>
+      <c r="H4" s="322"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="323"/>
-      <c r="C5" s="323"/>
-      <c r="D5" s="323"/>
-      <c r="E5" s="323"/>
-      <c r="F5" s="323"/>
-      <c r="G5" s="323"/>
-      <c r="H5" s="323"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="322"/>
+      <c r="D5" s="322"/>
+      <c r="E5" s="322"/>
+      <c r="F5" s="322"/>
+      <c r="G5" s="322"/>
+      <c r="H5" s="322"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="323"/>
-      <c r="C6" s="323"/>
-      <c r="D6" s="323"/>
-      <c r="E6" s="323"/>
-      <c r="F6" s="323"/>
-      <c r="G6" s="323"/>
-      <c r="H6" s="323"/>
+      <c r="B6" s="322"/>
+      <c r="C6" s="322"/>
+      <c r="D6" s="322"/>
+      <c r="E6" s="322"/>
+      <c r="F6" s="322"/>
+      <c r="G6" s="322"/>
+      <c r="H6" s="322"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="323"/>
-      <c r="C7" s="323"/>
-      <c r="D7" s="323"/>
-      <c r="E7" s="323"/>
-      <c r="F7" s="323"/>
-      <c r="G7" s="323"/>
-      <c r="H7" s="323"/>
+      <c r="B7" s="322"/>
+      <c r="C7" s="322"/>
+      <c r="D7" s="322"/>
+      <c r="E7" s="322"/>
+      <c r="F7" s="322"/>
+      <c r="G7" s="322"/>
+      <c r="H7" s="322"/>
       <c r="I7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="323"/>
-      <c r="C8" s="323"/>
-      <c r="D8" s="323"/>
-      <c r="E8" s="323"/>
-      <c r="F8" s="323"/>
-      <c r="G8" s="323"/>
-      <c r="H8" s="323"/>
+      <c r="B8" s="322"/>
+      <c r="C8" s="322"/>
+      <c r="D8" s="322"/>
+      <c r="E8" s="322"/>
+      <c r="F8" s="322"/>
+      <c r="G8" s="322"/>
+      <c r="H8" s="322"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="323"/>
-      <c r="C9" s="323"/>
-      <c r="D9" s="323"/>
-      <c r="E9" s="323"/>
-      <c r="F9" s="323"/>
-      <c r="G9" s="323"/>
-      <c r="H9" s="323"/>
+      <c r="B9" s="322"/>
+      <c r="C9" s="322"/>
+      <c r="D9" s="322"/>
+      <c r="E9" s="322"/>
+      <c r="F9" s="322"/>
+      <c r="G9" s="322"/>
+      <c r="H9" s="322"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="323"/>
-      <c r="C10" s="323"/>
-      <c r="D10" s="323"/>
-      <c r="E10" s="323"/>
-      <c r="F10" s="323"/>
-      <c r="G10" s="323"/>
-      <c r="H10" s="323"/>
+      <c r="B10" s="322"/>
+      <c r="C10" s="322"/>
+      <c r="D10" s="322"/>
+      <c r="E10" s="322"/>
+      <c r="F10" s="322"/>
+      <c r="G10" s="322"/>
+      <c r="H10" s="322"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="323"/>
-      <c r="C11" s="323"/>
-      <c r="D11" s="323"/>
-      <c r="E11" s="323"/>
-      <c r="F11" s="323"/>
-      <c r="G11" s="323"/>
-      <c r="H11" s="323"/>
+      <c r="B11" s="322"/>
+      <c r="C11" s="322"/>
+      <c r="D11" s="322"/>
+      <c r="E11" s="322"/>
+      <c r="F11" s="322"/>
+      <c r="G11" s="322"/>
+      <c r="H11" s="322"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="323"/>
-      <c r="C12" s="323"/>
-      <c r="D12" s="323"/>
-      <c r="E12" s="323"/>
-      <c r="F12" s="323"/>
-      <c r="G12" s="323"/>
-      <c r="H12" s="323"/>
+      <c r="B12" s="322"/>
+      <c r="C12" s="322"/>
+      <c r="D12" s="322"/>
+      <c r="E12" s="322"/>
+      <c r="F12" s="322"/>
+      <c r="G12" s="322"/>
+      <c r="H12" s="322"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="323"/>
-      <c r="C13" s="323"/>
-      <c r="D13" s="323"/>
-      <c r="E13" s="323"/>
-      <c r="F13" s="323"/>
-      <c r="G13" s="323"/>
-      <c r="H13" s="323"/>
+      <c r="B13" s="322"/>
+      <c r="C13" s="322"/>
+      <c r="D13" s="322"/>
+      <c r="E13" s="322"/>
+      <c r="F13" s="322"/>
+      <c r="G13" s="322"/>
+      <c r="H13" s="322"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="323"/>
-      <c r="C14" s="323"/>
-      <c r="D14" s="323"/>
-      <c r="E14" s="323"/>
-      <c r="F14" s="323"/>
-      <c r="G14" s="323"/>
-      <c r="H14" s="323"/>
+      <c r="B14" s="322"/>
+      <c r="C14" s="322"/>
+      <c r="D14" s="322"/>
+      <c r="E14" s="322"/>
+      <c r="F14" s="322"/>
+      <c r="G14" s="322"/>
+      <c r="H14" s="322"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="323"/>
-      <c r="C15" s="323"/>
-      <c r="D15" s="323"/>
-      <c r="E15" s="323"/>
-      <c r="F15" s="323"/>
-      <c r="G15" s="323"/>
-      <c r="H15" s="323"/>
+      <c r="B15" s="322"/>
+      <c r="C15" s="322"/>
+      <c r="D15" s="322"/>
+      <c r="E15" s="322"/>
+      <c r="F15" s="322"/>
+      <c r="G15" s="322"/>
+      <c r="H15" s="322"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="323"/>
-      <c r="C16" s="323"/>
-      <c r="D16" s="323"/>
-      <c r="E16" s="323"/>
-      <c r="F16" s="323"/>
-      <c r="G16" s="323"/>
-      <c r="H16" s="323"/>
+      <c r="B16" s="322"/>
+      <c r="C16" s="322"/>
+      <c r="D16" s="322"/>
+      <c r="E16" s="322"/>
+      <c r="F16" s="322"/>
+      <c r="G16" s="322"/>
+      <c r="H16" s="322"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="323"/>
-      <c r="C17" s="323"/>
-      <c r="D17" s="323"/>
-      <c r="E17" s="323"/>
-      <c r="F17" s="323"/>
-      <c r="G17" s="323"/>
-      <c r="H17" s="323"/>
+      <c r="B17" s="322"/>
+      <c r="C17" s="322"/>
+      <c r="D17" s="322"/>
+      <c r="E17" s="322"/>
+      <c r="F17" s="322"/>
+      <c r="G17" s="322"/>
+      <c r="H17" s="322"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="323"/>
-      <c r="C18" s="323"/>
-      <c r="D18" s="323"/>
-      <c r="E18" s="323"/>
-      <c r="F18" s="323"/>
-      <c r="G18" s="323"/>
-      <c r="H18" s="323"/>
+      <c r="B18" s="322"/>
+      <c r="C18" s="322"/>
+      <c r="D18" s="322"/>
+      <c r="E18" s="322"/>
+      <c r="F18" s="322"/>
+      <c r="G18" s="322"/>
+      <c r="H18" s="322"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="323"/>
-      <c r="C19" s="323"/>
-      <c r="D19" s="323"/>
-      <c r="E19" s="323"/>
-      <c r="F19" s="323"/>
-      <c r="G19" s="323"/>
-      <c r="H19" s="323"/>
+      <c r="B19" s="322"/>
+      <c r="C19" s="322"/>
+      <c r="D19" s="322"/>
+      <c r="E19" s="322"/>
+      <c r="F19" s="322"/>
+      <c r="G19" s="322"/>
+      <c r="H19" s="322"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="323"/>
-      <c r="C20" s="323"/>
-      <c r="D20" s="323"/>
-      <c r="E20" s="323"/>
-      <c r="F20" s="323"/>
-      <c r="G20" s="323"/>
-      <c r="H20" s="323"/>
+      <c r="B20" s="322"/>
+      <c r="C20" s="322"/>
+      <c r="D20" s="322"/>
+      <c r="E20" s="322"/>
+      <c r="F20" s="322"/>
+      <c r="G20" s="322"/>
+      <c r="H20" s="322"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="323"/>
-      <c r="C21" s="323"/>
-      <c r="D21" s="323"/>
-      <c r="E21" s="323"/>
-      <c r="F21" s="323"/>
-      <c r="G21" s="323"/>
-      <c r="H21" s="323"/>
+      <c r="B21" s="322"/>
+      <c r="C21" s="322"/>
+      <c r="D21" s="322"/>
+      <c r="E21" s="322"/>
+      <c r="F21" s="322"/>
+      <c r="G21" s="322"/>
+      <c r="H21" s="322"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="323"/>
-      <c r="C22" s="323"/>
-      <c r="D22" s="323"/>
-      <c r="E22" s="323"/>
-      <c r="F22" s="323"/>
-      <c r="G22" s="323"/>
-      <c r="H22" s="323"/>
+      <c r="B22" s="322"/>
+      <c r="C22" s="322"/>
+      <c r="D22" s="322"/>
+      <c r="E22" s="322"/>
+      <c r="F22" s="322"/>
+      <c r="G22" s="322"/>
+      <c r="H22" s="322"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="323"/>
-      <c r="C23" s="323"/>
-      <c r="D23" s="323"/>
-      <c r="E23" s="323"/>
-      <c r="F23" s="323"/>
-      <c r="G23" s="323"/>
-      <c r="H23" s="323"/>
+      <c r="B23" s="322"/>
+      <c r="C23" s="322"/>
+      <c r="D23" s="322"/>
+      <c r="E23" s="322"/>
+      <c r="F23" s="322"/>
+      <c r="G23" s="322"/>
+      <c r="H23" s="322"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="323"/>
-      <c r="C24" s="323"/>
-      <c r="D24" s="323"/>
-      <c r="E24" s="323"/>
-      <c r="F24" s="323"/>
-      <c r="G24" s="323"/>
-      <c r="H24" s="323"/>
+      <c r="B24" s="322"/>
+      <c r="C24" s="322"/>
+      <c r="D24" s="322"/>
+      <c r="E24" s="322"/>
+      <c r="F24" s="322"/>
+      <c r="G24" s="322"/>
+      <c r="H24" s="322"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="323"/>
-      <c r="C25" s="323"/>
-      <c r="D25" s="323"/>
-      <c r="E25" s="323"/>
-      <c r="F25" s="323"/>
-      <c r="G25" s="323"/>
-      <c r="H25" s="323"/>
+      <c r="B25" s="322"/>
+      <c r="C25" s="322"/>
+      <c r="D25" s="322"/>
+      <c r="E25" s="322"/>
+      <c r="F25" s="322"/>
+      <c r="G25" s="322"/>
+      <c r="H25" s="322"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="323"/>
-      <c r="C26" s="323"/>
-      <c r="D26" s="323"/>
-      <c r="E26" s="323"/>
-      <c r="F26" s="323"/>
-      <c r="G26" s="323"/>
-      <c r="H26" s="323"/>
+      <c r="B26" s="322"/>
+      <c r="C26" s="322"/>
+      <c r="D26" s="322"/>
+      <c r="E26" s="322"/>
+      <c r="F26" s="322"/>
+      <c r="G26" s="322"/>
+      <c r="H26" s="322"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="323"/>
-      <c r="C27" s="323"/>
-      <c r="D27" s="323"/>
-      <c r="E27" s="323"/>
-      <c r="F27" s="323"/>
-      <c r="G27" s="323"/>
-      <c r="H27" s="323"/>
+      <c r="B27" s="322"/>
+      <c r="C27" s="322"/>
+      <c r="D27" s="322"/>
+      <c r="E27" s="322"/>
+      <c r="F27" s="322"/>
+      <c r="G27" s="322"/>
+      <c r="H27" s="322"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="323"/>
-      <c r="C28" s="323"/>
-      <c r="D28" s="323"/>
-      <c r="E28" s="323"/>
-      <c r="F28" s="323"/>
-      <c r="G28" s="323"/>
-      <c r="H28" s="323"/>
+      <c r="B28" s="322"/>
+      <c r="C28" s="322"/>
+      <c r="D28" s="322"/>
+      <c r="E28" s="322"/>
+      <c r="F28" s="322"/>
+      <c r="G28" s="322"/>
+      <c r="H28" s="322"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="323"/>
-      <c r="C29" s="323"/>
-      <c r="D29" s="323"/>
-      <c r="E29" s="323"/>
-      <c r="F29" s="323"/>
-      <c r="G29" s="323"/>
-      <c r="H29" s="323"/>
+      <c r="B29" s="322"/>
+      <c r="C29" s="322"/>
+      <c r="D29" s="322"/>
+      <c r="E29" s="322"/>
+      <c r="F29" s="322"/>
+      <c r="G29" s="322"/>
+      <c r="H29" s="322"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="323"/>
-      <c r="C30" s="323"/>
-      <c r="D30" s="323"/>
-      <c r="E30" s="323"/>
-      <c r="F30" s="323"/>
-      <c r="G30" s="323"/>
-      <c r="H30" s="323"/>
+      <c r="B30" s="322"/>
+      <c r="C30" s="322"/>
+      <c r="D30" s="322"/>
+      <c r="E30" s="322"/>
+      <c r="F30" s="322"/>
+      <c r="G30" s="322"/>
+      <c r="H30" s="322"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="323"/>
-      <c r="C31" s="323"/>
-      <c r="D31" s="323"/>
-      <c r="E31" s="323"/>
-      <c r="F31" s="323"/>
-      <c r="G31" s="323"/>
-      <c r="H31" s="323"/>
+      <c r="B31" s="322"/>
+      <c r="C31" s="322"/>
+      <c r="D31" s="322"/>
+      <c r="E31" s="322"/>
+      <c r="F31" s="322"/>
+      <c r="G31" s="322"/>
+      <c r="H31" s="322"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="323"/>
-      <c r="C32" s="323"/>
-      <c r="D32" s="323"/>
-      <c r="E32" s="323"/>
-      <c r="F32" s="323"/>
-      <c r="G32" s="323"/>
-      <c r="H32" s="323"/>
+      <c r="B32" s="322"/>
+      <c r="C32" s="322"/>
+      <c r="D32" s="322"/>
+      <c r="E32" s="322"/>
+      <c r="F32" s="322"/>
+      <c r="G32" s="322"/>
+      <c r="H32" s="322"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="323"/>
-      <c r="C33" s="323"/>
-      <c r="D33" s="323"/>
-      <c r="E33" s="323"/>
-      <c r="F33" s="323"/>
-      <c r="G33" s="323"/>
-      <c r="H33" s="323"/>
+      <c r="B33" s="322"/>
+      <c r="C33" s="322"/>
+      <c r="D33" s="322"/>
+      <c r="E33" s="322"/>
+      <c r="F33" s="322"/>
+      <c r="G33" s="322"/>
+      <c r="H33" s="322"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="323"/>
-      <c r="C34" s="323"/>
-      <c r="D34" s="323"/>
-      <c r="E34" s="323"/>
-      <c r="F34" s="323"/>
-      <c r="G34" s="323"/>
-      <c r="H34" s="323"/>
+      <c r="B34" s="322"/>
+      <c r="C34" s="322"/>
+      <c r="D34" s="322"/>
+      <c r="E34" s="322"/>
+      <c r="F34" s="322"/>
+      <c r="G34" s="322"/>
+      <c r="H34" s="322"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="323"/>
-      <c r="C35" s="323"/>
-      <c r="D35" s="323"/>
-      <c r="E35" s="323"/>
-      <c r="F35" s="323"/>
-      <c r="G35" s="323"/>
-      <c r="H35" s="323"/>
+      <c r="B35" s="322"/>
+      <c r="C35" s="322"/>
+      <c r="D35" s="322"/>
+      <c r="E35" s="322"/>
+      <c r="F35" s="322"/>
+      <c r="G35" s="322"/>
+      <c r="H35" s="322"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="323"/>
-      <c r="C36" s="323"/>
-      <c r="D36" s="323"/>
-      <c r="E36" s="323"/>
-      <c r="F36" s="323"/>
-      <c r="G36" s="323"/>
-      <c r="H36" s="323"/>
+      <c r="B36" s="322"/>
+      <c r="C36" s="322"/>
+      <c r="D36" s="322"/>
+      <c r="E36" s="322"/>
+      <c r="F36" s="322"/>
+      <c r="G36" s="322"/>
+      <c r="H36" s="322"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="323"/>
-      <c r="C37" s="323"/>
-      <c r="D37" s="323"/>
-      <c r="E37" s="323"/>
-      <c r="F37" s="323"/>
-      <c r="G37" s="323"/>
-      <c r="H37" s="323"/>
+      <c r="B37" s="322"/>
+      <c r="C37" s="322"/>
+      <c r="D37" s="322"/>
+      <c r="E37" s="322"/>
+      <c r="F37" s="322"/>
+      <c r="G37" s="322"/>
+      <c r="H37" s="322"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="323"/>
-      <c r="C38" s="323"/>
-      <c r="D38" s="323"/>
-      <c r="E38" s="323"/>
-      <c r="F38" s="323"/>
-      <c r="G38" s="323"/>
-      <c r="H38" s="323"/>
+      <c r="B38" s="322"/>
+      <c r="C38" s="322"/>
+      <c r="D38" s="322"/>
+      <c r="E38" s="322"/>
+      <c r="F38" s="322"/>
+      <c r="G38" s="322"/>
+      <c r="H38" s="322"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="323"/>
-      <c r="C39" s="323"/>
-      <c r="D39" s="323"/>
-      <c r="E39" s="323"/>
-      <c r="F39" s="323"/>
-      <c r="G39" s="323"/>
-      <c r="H39" s="323"/>
+      <c r="B39" s="322"/>
+      <c r="C39" s="322"/>
+      <c r="D39" s="322"/>
+      <c r="E39" s="322"/>
+      <c r="F39" s="322"/>
+      <c r="G39" s="322"/>
+      <c r="H39" s="322"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="323"/>
-      <c r="C40" s="323"/>
-      <c r="D40" s="323"/>
-      <c r="E40" s="323"/>
-      <c r="F40" s="323"/>
-      <c r="G40" s="323"/>
-      <c r="H40" s="323"/>
+      <c r="B40" s="322"/>
+      <c r="C40" s="322"/>
+      <c r="D40" s="322"/>
+      <c r="E40" s="322"/>
+      <c r="F40" s="322"/>
+      <c r="G40" s="322"/>
+      <c r="H40" s="322"/>
     </row>
     <row r="41" customFormat="false" ht="6.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="323"/>
-      <c r="C41" s="323"/>
-      <c r="D41" s="323"/>
-      <c r="E41" s="323"/>
-      <c r="F41" s="323"/>
-      <c r="G41" s="323"/>
-      <c r="H41" s="323"/>
+      <c r="B41" s="322"/>
+      <c r="C41" s="322"/>
+      <c r="D41" s="322"/>
+      <c r="E41" s="322"/>
+      <c r="F41" s="322"/>
+      <c r="G41" s="322"/>
+      <c r="H41" s="322"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="323"/>
-      <c r="C42" s="323"/>
-      <c r="D42" s="323"/>
-      <c r="E42" s="323"/>
-      <c r="F42" s="323"/>
-      <c r="G42" s="323"/>
-      <c r="H42" s="323"/>
+      <c r="B42" s="322"/>
+      <c r="C42" s="322"/>
+      <c r="D42" s="322"/>
+      <c r="E42" s="322"/>
+      <c r="F42" s="322"/>
+      <c r="G42" s="322"/>
+      <c r="H42" s="322"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="323"/>
-      <c r="C43" s="323"/>
-      <c r="D43" s="323"/>
-      <c r="E43" s="323"/>
-      <c r="F43" s="323"/>
-      <c r="G43" s="323"/>
-      <c r="H43" s="323"/>
+      <c r="B43" s="322"/>
+      <c r="C43" s="322"/>
+      <c r="D43" s="322"/>
+      <c r="E43" s="322"/>
+      <c r="F43" s="322"/>
+      <c r="G43" s="322"/>
+      <c r="H43" s="322"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="323"/>
-      <c r="C44" s="323"/>
-      <c r="D44" s="323"/>
-      <c r="E44" s="323"/>
-      <c r="F44" s="323"/>
-      <c r="G44" s="323"/>
-      <c r="H44" s="323"/>
+      <c r="B44" s="322"/>
+      <c r="C44" s="322"/>
+      <c r="D44" s="322"/>
+      <c r="E44" s="322"/>
+      <c r="F44" s="322"/>
+      <c r="G44" s="322"/>
+      <c r="H44" s="322"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="323"/>
-      <c r="C45" s="323"/>
-      <c r="D45" s="323"/>
-      <c r="E45" s="323"/>
-      <c r="F45" s="323"/>
-      <c r="G45" s="323"/>
-      <c r="H45" s="323"/>
+      <c r="B45" s="322"/>
+      <c r="C45" s="322"/>
+      <c r="D45" s="322"/>
+      <c r="E45" s="322"/>
+      <c r="F45" s="322"/>
+      <c r="G45" s="322"/>
+      <c r="H45" s="322"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="323"/>
-      <c r="C46" s="323"/>
-      <c r="D46" s="323"/>
-      <c r="E46" s="323"/>
-      <c r="F46" s="323"/>
-      <c r="G46" s="323"/>
-      <c r="H46" s="323"/>
+      <c r="B46" s="322"/>
+      <c r="C46" s="322"/>
+      <c r="D46" s="322"/>
+      <c r="E46" s="322"/>
+      <c r="F46" s="322"/>
+      <c r="G46" s="322"/>
+      <c r="H46" s="322"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="323"/>
-      <c r="C47" s="323"/>
-      <c r="D47" s="323"/>
-      <c r="E47" s="323"/>
-      <c r="F47" s="323"/>
-      <c r="G47" s="323"/>
-      <c r="H47" s="323"/>
+      <c r="B47" s="322"/>
+      <c r="C47" s="322"/>
+      <c r="D47" s="322"/>
+      <c r="E47" s="322"/>
+      <c r="F47" s="322"/>
+      <c r="G47" s="322"/>
+      <c r="H47" s="322"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="323"/>
-      <c r="C48" s="323"/>
-      <c r="D48" s="323"/>
-      <c r="E48" s="323"/>
-      <c r="F48" s="323"/>
-      <c r="G48" s="323"/>
-      <c r="H48" s="323"/>
+      <c r="B48" s="322"/>
+      <c r="C48" s="322"/>
+      <c r="D48" s="322"/>
+      <c r="E48" s="322"/>
+      <c r="F48" s="322"/>
+      <c r="G48" s="322"/>
+      <c r="H48" s="322"/>
     </row>
     <row r="49" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="323"/>
-      <c r="C49" s="323"/>
-      <c r="D49" s="323"/>
-      <c r="E49" s="323"/>
-      <c r="F49" s="323"/>
-      <c r="G49" s="323"/>
-      <c r="H49" s="323"/>
+      <c r="B49" s="322"/>
+      <c r="C49" s="322"/>
+      <c r="D49" s="322"/>
+      <c r="E49" s="322"/>
+      <c r="F49" s="322"/>
+      <c r="G49" s="322"/>
+      <c r="H49" s="322"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="323"/>
-      <c r="C50" s="323"/>
-      <c r="D50" s="323"/>
-      <c r="E50" s="323"/>
-      <c r="F50" s="323"/>
-      <c r="G50" s="323"/>
-      <c r="H50" s="323"/>
+      <c r="B50" s="322"/>
+      <c r="C50" s="322"/>
+      <c r="D50" s="322"/>
+      <c r="E50" s="322"/>
+      <c r="F50" s="322"/>
+      <c r="G50" s="322"/>
+      <c r="H50" s="322"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="323"/>
-      <c r="C51" s="323"/>
-      <c r="D51" s="323"/>
-      <c r="E51" s="323"/>
-      <c r="F51" s="323"/>
-      <c r="G51" s="323"/>
-      <c r="H51" s="323"/>
+      <c r="B51" s="322"/>
+      <c r="C51" s="322"/>
+      <c r="D51" s="322"/>
+      <c r="E51" s="322"/>
+      <c r="F51" s="322"/>
+      <c r="G51" s="322"/>
+      <c r="H51" s="322"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="323"/>
-      <c r="C52" s="323"/>
-      <c r="D52" s="323"/>
-      <c r="E52" s="323"/>
-      <c r="F52" s="323"/>
-      <c r="G52" s="323"/>
-      <c r="H52" s="323"/>
+      <c r="B52" s="322"/>
+      <c r="C52" s="322"/>
+      <c r="D52" s="322"/>
+      <c r="E52" s="322"/>
+      <c r="F52" s="322"/>
+      <c r="G52" s="322"/>
+      <c r="H52" s="322"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="323"/>
-      <c r="C53" s="323"/>
-      <c r="D53" s="323"/>
-      <c r="E53" s="323"/>
-      <c r="F53" s="323"/>
-      <c r="G53" s="323"/>
-      <c r="H53" s="323"/>
+      <c r="B53" s="322"/>
+      <c r="C53" s="322"/>
+      <c r="D53" s="322"/>
+      <c r="E53" s="322"/>
+      <c r="F53" s="322"/>
+      <c r="G53" s="322"/>
+      <c r="H53" s="322"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="323"/>
-      <c r="C54" s="323"/>
-      <c r="D54" s="323"/>
-      <c r="E54" s="323"/>
-      <c r="F54" s="323"/>
-      <c r="G54" s="323"/>
-      <c r="H54" s="323"/>
+      <c r="B54" s="322"/>
+      <c r="C54" s="322"/>
+      <c r="D54" s="322"/>
+      <c r="E54" s="322"/>
+      <c r="F54" s="322"/>
+      <c r="G54" s="322"/>
+      <c r="H54" s="322"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="323"/>
-      <c r="C55" s="323"/>
-      <c r="D55" s="323"/>
-      <c r="E55" s="323"/>
-      <c r="F55" s="323"/>
-      <c r="G55" s="323"/>
-      <c r="H55" s="323"/>
+      <c r="B55" s="322"/>
+      <c r="C55" s="322"/>
+      <c r="D55" s="322"/>
+      <c r="E55" s="322"/>
+      <c r="F55" s="322"/>
+      <c r="G55" s="322"/>
+      <c r="H55" s="322"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="323"/>
-      <c r="C56" s="323"/>
-      <c r="D56" s="323"/>
-      <c r="E56" s="323"/>
-      <c r="F56" s="323"/>
-      <c r="G56" s="323"/>
-      <c r="H56" s="323"/>
+      <c r="B56" s="322"/>
+      <c r="C56" s="322"/>
+      <c r="D56" s="322"/>
+      <c r="E56" s="322"/>
+      <c r="F56" s="322"/>
+      <c r="G56" s="322"/>
+      <c r="H56" s="322"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="323"/>
-      <c r="C57" s="323"/>
-      <c r="D57" s="323"/>
-      <c r="E57" s="323"/>
-      <c r="F57" s="323"/>
-      <c r="G57" s="323"/>
-      <c r="H57" s="323"/>
+      <c r="B57" s="322"/>
+      <c r="C57" s="322"/>
+      <c r="D57" s="322"/>
+      <c r="E57" s="322"/>
+      <c r="F57" s="322"/>
+      <c r="G57" s="322"/>
+      <c r="H57" s="322"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="323"/>
-      <c r="C58" s="323"/>
-      <c r="D58" s="323"/>
-      <c r="E58" s="323"/>
-      <c r="F58" s="323"/>
-      <c r="G58" s="323"/>
-      <c r="H58" s="323"/>
+      <c r="B58" s="322"/>
+      <c r="C58" s="322"/>
+      <c r="D58" s="322"/>
+      <c r="E58" s="322"/>
+      <c r="F58" s="322"/>
+      <c r="G58" s="322"/>
+      <c r="H58" s="322"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="323"/>
-      <c r="C59" s="323"/>
-      <c r="D59" s="323"/>
-      <c r="E59" s="323"/>
-      <c r="F59" s="323"/>
-      <c r="G59" s="323"/>
-      <c r="H59" s="323"/>
+      <c r="B59" s="322"/>
+      <c r="C59" s="322"/>
+      <c r="D59" s="322"/>
+      <c r="E59" s="322"/>
+      <c r="F59" s="322"/>
+      <c r="G59" s="322"/>
+      <c r="H59" s="322"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="323"/>
-      <c r="C60" s="323"/>
-      <c r="D60" s="323"/>
-      <c r="E60" s="323"/>
-      <c r="F60" s="323"/>
-      <c r="G60" s="323"/>
-      <c r="H60" s="323"/>
+      <c r="B60" s="322"/>
+      <c r="C60" s="322"/>
+      <c r="D60" s="322"/>
+      <c r="E60" s="322"/>
+      <c r="F60" s="322"/>
+      <c r="G60" s="322"/>
+      <c r="H60" s="322"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="151"/>
@@ -16962,7 +16950,7 @@
       <c r="E61" s="152"/>
       <c r="F61" s="152"/>
       <c r="G61" s="152"/>
-      <c r="H61" s="371"/>
+      <c r="H61" s="370"/>
     </row>
   </sheetData>
   <mergeCells count="59">

</xml_diff>

<commit_message>
Fix formatting and typos near valmistumisvuosi on page 2 of energiatodistus pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -1596,7 +1596,7 @@
     <numFmt numFmtId="169" formatCode="[$-40B]0"/>
     <numFmt numFmtId="170" formatCode="[$-40B]0.00"/>
     <numFmt numFmtId="171" formatCode="[$-40B]General"/>
-    <numFmt numFmtId="172" formatCode="[$-409]@"/>
+    <numFmt numFmtId="172" formatCode="[$-40B]0.0"/>
     <numFmt numFmtId="173" formatCode="[$-40B]0\.0"/>
     <numFmt numFmtId="174" formatCode="@"/>
     <numFmt numFmtId="175" formatCode="0"/>
@@ -2380,7 +2380,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2851,8 +2851,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2887,8 +2887,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -6364,9 +6364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>244080</xdr:colOff>
+      <xdr:colOff>243720</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6380,7 +6380,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="754200" cy="210960"/>
+          <a:ext cx="753840" cy="210600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6401,9 +6401,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>144000</xdr:colOff>
+      <xdr:colOff>143640</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6417,7 +6417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1097640" cy="210960"/>
+          <a:ext cx="1097280" cy="210600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6438,9 +6438,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>17280</xdr:colOff>
+      <xdr:colOff>16920</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6454,7 +6454,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1404360" cy="210960"/>
+          <a:ext cx="1404000" cy="210600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6475,9 +6475,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>341280</xdr:colOff>
+      <xdr:colOff>340920</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6491,7 +6491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1728360" cy="210960"/>
+          <a:ext cx="1728000" cy="210600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6512,9 +6512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>214560</xdr:colOff>
+      <xdr:colOff>214200</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>271440</xdr:rowOff>
+      <xdr:rowOff>271080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6528,7 +6528,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2035440" cy="223920"/>
+          <a:ext cx="2035080" cy="223560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6549,9 +6549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>157680</xdr:colOff>
+      <xdr:colOff>157320</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6565,7 +6565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2371680" cy="210960"/>
+          <a:ext cx="2371320" cy="210600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6586,9 +6586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>97920</xdr:colOff>
+      <xdr:colOff>97560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>258480</xdr:rowOff>
+      <xdr:rowOff>258120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6598,7 +6598,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530400"/>
-          <a:ext cx="2684520" cy="209880"/>
+          <a:ext cx="2684160" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6967,9 +6967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>297360</xdr:colOff>
+      <xdr:colOff>297000</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>97920</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6979,7 +6979,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6983640" cy="10553400"/>
+          <a:ext cx="6983280" cy="10553040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7107,9 +7107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>422280</xdr:colOff>
+      <xdr:colOff>421920</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>291960</xdr:rowOff>
+      <xdr:rowOff>291600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7123,7 +7123,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5087520" y="5274720"/>
-          <a:ext cx="1122120" cy="255240"/>
+          <a:ext cx="1121760" cy="254880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7149,9 +7149,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>144360</xdr:colOff>
+      <xdr:colOff>144000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7161,7 +7161,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="201240" y="10549800"/>
-          <a:ext cx="7018920" cy="253440"/>
+          <a:ext cx="7018560" cy="253080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7216,13 +7216,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>104040</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1009080</xdr:colOff>
+      <xdr:colOff>1008720</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7232,7 +7232,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="396000" y="10928880"/>
-          <a:ext cx="7086240" cy="259920"/>
+          <a:ext cx="7085880" cy="259560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7291,9 +7291,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1012680</xdr:colOff>
+      <xdr:colOff>1012320</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7303,7 +7303,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="290520" y="11094480"/>
-          <a:ext cx="7045920" cy="254880"/>
+          <a:ext cx="7045560" cy="254520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7362,9 +7362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>29160</xdr:colOff>
+      <xdr:colOff>28800</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7374,7 +7374,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="241920" y="9930960"/>
-          <a:ext cx="6885000" cy="254160"/>
+          <a:ext cx="6884640" cy="253800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7433,9 +7433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>47880</xdr:colOff>
+      <xdr:colOff>47520</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>55080</xdr:rowOff>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7445,7 +7445,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="170640" y="10200240"/>
-          <a:ext cx="6981480" cy="354960"/>
+          <a:ext cx="6981120" cy="354600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7504,9 +7504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57240</xdr:colOff>
+      <xdr:colOff>56880</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>63000</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7516,7 +7516,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="163440" y="10335960"/>
-          <a:ext cx="6990480" cy="366120"/>
+          <a:ext cx="6990120" cy="365760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7575,9 +7575,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
+      <xdr:colOff>76680</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7587,7 +7587,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="90720" y="9993600"/>
-          <a:ext cx="7030800" cy="366120"/>
+          <a:ext cx="7030440" cy="365760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11133,8 +11133,8 @@
   </sheetPr>
   <dimension ref="B2:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11205,12 +11205,12 @@
       <c r="F3" s="159"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="160"/>
       <c r="C4" s="161" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="161"/>
+      <c r="D4" s="162"/>
       <c r="E4" s="162"/>
       <c r="F4" s="162"/>
       <c r="G4" s="162"/>
@@ -11968,10 +11968,9 @@
       <c r="G67" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="D4:G4"/>
     <mergeCell ref="D28:G28"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="E36:G36"/>
@@ -12471,7 +12470,7 @@
   </sheetPr>
   <dimension ref="B2:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AE-293 fix more colors in xlsx template
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) etusivu" sheetId="1" state="visible" r:id="rId2"/>
@@ -2383,7 +2383,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2862,7 +2862,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -3214,7 +3214,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -6375,9 +6375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>242640</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6391,7 +6391,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="753120" cy="209880"/>
+          <a:ext cx="752760" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6412,9 +6412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
+      <xdr:colOff>142560</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6428,7 +6428,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1096560" cy="209880"/>
+          <a:ext cx="1096200" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6449,9 +6449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>16200</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6465,7 +6465,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1403280" cy="209880"/>
+          <a:ext cx="1402920" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6486,9 +6486,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>340200</xdr:colOff>
+      <xdr:colOff>339840</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6502,7 +6502,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1727280" cy="209880"/>
+          <a:ext cx="1726920" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6523,9 +6523,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>213480</xdr:colOff>
+      <xdr:colOff>213120</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>270360</xdr:rowOff>
+      <xdr:rowOff>270000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6539,7 +6539,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2034360" cy="222840"/>
+          <a:ext cx="2034000" cy="222480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6560,9 +6560,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>156600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6576,7 +6576,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2370600" cy="209880"/>
+          <a:ext cx="2370240" cy="209520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6597,9 +6597,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>96840</xdr:colOff>
+      <xdr:colOff>96480</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>257040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6609,7 +6609,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530400"/>
-          <a:ext cx="2683440" cy="208800"/>
+          <a:ext cx="2683080" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6978,9 +6978,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>296280</xdr:colOff>
+      <xdr:colOff>295920</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6990,7 +6990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6982560" cy="10552320"/>
+          <a:ext cx="6982200" cy="10551960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7118,9 +7118,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>421200</xdr:colOff>
+      <xdr:colOff>420840</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>290880</xdr:rowOff>
+      <xdr:rowOff>290520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7134,7 +7134,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5087520" y="5274720"/>
-          <a:ext cx="1121040" cy="254160"/>
+          <a:ext cx="1120680" cy="253800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7160,9 +7160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>143280</xdr:colOff>
+      <xdr:colOff>142920</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7172,7 +7172,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="201240" y="10549800"/>
-          <a:ext cx="7017840" cy="252360"/>
+          <a:ext cx="7017480" cy="252000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7231,9 +7231,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1008000</xdr:colOff>
+      <xdr:colOff>1007640</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7243,7 +7243,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="396000" y="10928880"/>
-          <a:ext cx="7085160" cy="258840"/>
+          <a:ext cx="7084800" cy="258480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7302,9 +7302,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1011600</xdr:colOff>
+      <xdr:colOff>1011240</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>47520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7314,7 +7314,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="290520" y="11094480"/>
-          <a:ext cx="7044840" cy="253800"/>
+          <a:ext cx="7044480" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7373,9 +7373,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>28080</xdr:colOff>
+      <xdr:colOff>27720</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7385,7 +7385,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="241920" y="9930960"/>
-          <a:ext cx="6883920" cy="253080"/>
+          <a:ext cx="6883560" cy="252720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7444,9 +7444,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
+      <xdr:colOff>46440</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7456,7 +7456,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="170640" y="10200240"/>
-          <a:ext cx="6980400" cy="353880"/>
+          <a:ext cx="6980040" cy="353520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7515,9 +7515,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>56160</xdr:colOff>
+      <xdr:colOff>55800</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7527,7 +7527,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="163440" y="10335960"/>
-          <a:ext cx="6989400" cy="365040"/>
+          <a:ext cx="6989040" cy="364680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7586,9 +7586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>75600</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>61560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7598,7 +7598,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="90720" y="9993600"/>
-          <a:ext cx="7029720" cy="365040"/>
+          <a:ext cx="7029360" cy="364680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11145,8 +11145,8 @@
   </sheetPr>
   <dimension ref="B2:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12582,20 +12582,20 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="162"/>
-      <c r="C7" s="165" t="s">
+      <c r="C7" s="253" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="253"/>
+      <c r="D7" s="165"/>
       <c r="E7" s="254"/>
       <c r="F7" s="177"/>
       <c r="G7" s="167"/>
     </row>
     <row r="8" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="162"/>
-      <c r="C8" s="165" t="s">
+      <c r="C8" s="253" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="253"/>
+      <c r="D8" s="165"/>
       <c r="E8" s="255"/>
       <c r="F8" s="194"/>
       <c r="G8" s="196"/>
@@ -15075,7 +15075,7 @@
   </sheetPr>
   <dimension ref="B1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AE-348 add uuden rakennuksen e-luvun vaatimus to energiatodistus pdf
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="208">
   <si>
     <t xml:space="preserve">ENERGIATODISTUS 2018</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ei rajapinnasta</t>
   </si>
   <si>
     <t xml:space="preserve">Todistuksen laatija:</t>
@@ -1721,13 +1718,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF4000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF009EE0"/>
@@ -1760,6 +1750,13 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF4000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2482,7 +2479,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2526,7 +2523,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2534,7 +2531,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2578,7 +2575,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2590,7 +2587,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2702,7 +2699,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2730,11 +2727,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -2742,7 +2739,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -2750,39 +2747,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="8" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="9" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2814,11 +2811,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2838,11 +2835,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -3174,11 +3171,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -3266,7 +3263,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -3342,7 +3339,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3402,7 +3399,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3606,7 +3603,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3698,7 +3695,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6383,9 +6380,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>241920</xdr:colOff>
+      <xdr:colOff>241560</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6399,7 +6396,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="752040" cy="208800"/>
+          <a:ext cx="751680" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6420,9 +6417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>141840</xdr:colOff>
+      <xdr:colOff>141480</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6436,7 +6433,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1095480" cy="208800"/>
+          <a:ext cx="1095120" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6457,9 +6454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6473,7 +6470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1402200" cy="208800"/>
+          <a:ext cx="1401840" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6494,9 +6491,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>339120</xdr:colOff>
+      <xdr:colOff>338760</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6510,7 +6507,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1726200" cy="208800"/>
+          <a:ext cx="1725840" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6531,9 +6528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>212400</xdr:colOff>
+      <xdr:colOff>212040</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>269280</xdr:rowOff>
+      <xdr:rowOff>268920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6547,7 +6544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2033280" cy="221760"/>
+          <a:ext cx="2032920" cy="221400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6568,9 +6565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>155520</xdr:colOff>
+      <xdr:colOff>155160</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6584,7 +6581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2369520" cy="208800"/>
+          <a:ext cx="2369160" cy="208440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6605,9 +6602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>95760</xdr:colOff>
+      <xdr:colOff>95400</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>256320</xdr:rowOff>
+      <xdr:rowOff>255960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6617,7 +6614,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530400"/>
-          <a:ext cx="2682360" cy="207720"/>
+          <a:ext cx="2682000" cy="207360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6986,9 +6983,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>295200</xdr:colOff>
+      <xdr:colOff>294840</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6998,7 +6995,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6981480" cy="10551240"/>
+          <a:ext cx="6981120" cy="10550880"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7131,9 +7128,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>142200</xdr:colOff>
+      <xdr:colOff>141840</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7143,7 +7140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="201240" y="10549800"/>
-          <a:ext cx="7016760" cy="251280"/>
+          <a:ext cx="7016400" cy="250920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7202,9 +7199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1006920</xdr:colOff>
+      <xdr:colOff>1006560</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>119520</xdr:rowOff>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7214,7 +7211,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="396000" y="10928880"/>
-          <a:ext cx="7084080" cy="257760"/>
+          <a:ext cx="7083720" cy="257400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7273,9 +7270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1010520</xdr:colOff>
+      <xdr:colOff>1010160</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7285,7 +7282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="290520" y="11094480"/>
-          <a:ext cx="7043760" cy="252720"/>
+          <a:ext cx="7043400" cy="252360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7344,9 +7341,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>26640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>116640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7356,7 +7353,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="241920" y="9930960"/>
-          <a:ext cx="6882840" cy="252000"/>
+          <a:ext cx="6882480" cy="251640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7415,9 +7412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>45360</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7427,7 +7424,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="170640" y="10200240"/>
-          <a:ext cx="6979320" cy="352800"/>
+          <a:ext cx="6978960" cy="352440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7486,9 +7483,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>55080</xdr:colOff>
+      <xdr:colOff>54720</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7498,7 +7495,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="163440" y="10335960"/>
-          <a:ext cx="6988320" cy="363960"/>
+          <a:ext cx="6987960" cy="363600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7557,9 +7554,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>74880</xdr:colOff>
+      <xdr:colOff>74520</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7569,7 +7566,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="90720" y="9993600"/>
-          <a:ext cx="7028640" cy="363960"/>
+          <a:ext cx="7028280" cy="363600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7624,8 +7621,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
+    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8759,9 +8756,7 @@
       <c r="L37" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="M37" s="70" t="s">
-        <v>16</v>
-      </c>
+      <c r="M37" s="70"/>
       <c r="N37" s="71"/>
       <c r="O37" s="63"/>
       <c r="P37" s="59"/>
@@ -8827,7 +8822,7 @@
     <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -8837,7 +8832,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="76"/>
@@ -8888,7 +8883,7 @@
     <row r="44" customFormat="false" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
@@ -8963,7 +8958,7 @@
     </row>
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48" s="86"/>
       <c r="D48" s="86"/>
@@ -8974,7 +8969,7 @@
       <c r="I48" s="86"/>
       <c r="J48" s="86"/>
       <c r="K48" s="87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L48" s="88"/>
       <c r="M48" s="88"/>
@@ -9212,7 +9207,7 @@
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="96"/>
       <c r="C2" s="97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="97"/>
       <c r="E2" s="97"/>
@@ -9241,7 +9236,7 @@
     <row r="3" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="98"/>
       <c r="C3" s="99" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="99"/>
       <c r="E3" s="100"/>
@@ -9297,7 +9292,7 @@
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="102"/>
       <c r="C5" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -9326,7 +9321,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="102"/>
       <c r="C6" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -9356,7 +9351,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="102"/>
       <c r="C7" s="107" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="108"/>
       <c r="E7" s="108"/>
@@ -9413,19 +9408,19 @@
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="96"/>
       <c r="C9" s="114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="114"/>
       <c r="E9" s="114"/>
       <c r="F9" s="115" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="115"/>
       <c r="H9" s="116" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="116" t="s">
         <v>29</v>
-      </c>
-      <c r="I9" s="116" t="s">
-        <v>30</v>
       </c>
       <c r="J9" s="116"/>
       <c r="L9" s="0"/>
@@ -9505,16 +9500,16 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="118" t="s">
+      <c r="H12" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="119" t="s">
+      <c r="I12" s="117" t="s">
         <v>33</v>
-      </c>
-      <c r="I12" s="117" t="s">
-        <v>34</v>
       </c>
       <c r="J12" s="117"/>
       <c r="L12" s="0"/>
@@ -9564,7 +9559,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="102"/>
       <c r="C14" s="124" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="124"/>
       <c r="E14" s="4"/>
@@ -9593,7 +9588,7 @@
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="102"/>
       <c r="C15" s="124" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="124"/>
       <c r="E15" s="4"/>
@@ -9622,7 +9617,7 @@
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="102"/>
       <c r="C16" s="124" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="124"/>
       <c r="E16" s="4"/>
@@ -9651,7 +9646,7 @@
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="102"/>
       <c r="C17" s="124" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="124"/>
       <c r="E17" s="4"/>
@@ -9680,7 +9675,7 @@
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="102"/>
       <c r="C18" s="124" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="124"/>
       <c r="E18" s="4"/>
@@ -9736,7 +9731,7 @@
     <row r="20" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="130"/>
       <c r="C20" s="131" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="131"/>
       <c r="E20" s="131"/>
@@ -9765,7 +9760,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="98"/>
       <c r="C21" s="99" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="99"/>
       <c r="E21" s="100"/>
@@ -9821,7 +9816,7 @@
     <row r="23" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="102"/>
       <c r="C23" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="4"/>
@@ -9878,7 +9873,7 @@
     <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="102"/>
       <c r="C25" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="4"/>
@@ -9988,7 +9983,7 @@
     <row r="29" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="102"/>
       <c r="C29" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="4"/>
@@ -10044,7 +10039,7 @@
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="102"/>
       <c r="C31" s="149" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" s="149"/>
       <c r="E31" s="149"/>
@@ -10181,7 +10176,7 @@
     <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="153"/>
       <c r="C36" s="154" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" s="154"/>
       <c r="E36" s="154"/>
@@ -10210,7 +10205,7 @@
     <row r="37" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="98"/>
       <c r="C37" s="99" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="99"/>
       <c r="E37" s="100"/>
@@ -10751,7 +10746,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="158" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C57" s="158"/>
       <c r="D57" s="158"/>
@@ -11131,7 +11126,7 @@
   <sheetData>
     <row r="2" s="95" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="160" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="160"/>
       <c r="D2" s="160"/>
@@ -11180,7 +11175,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="161"/>
       <c r="C3" s="162" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="163"/>
       <c r="E3" s="163"/>
@@ -11190,7 +11185,7 @@
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="164"/>
       <c r="C4" s="165" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="166"/>
       <c r="E4" s="166"/>
@@ -11205,21 +11200,21 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="164"/>
       <c r="C5" s="165" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="167"/>
       <c r="E5" s="165" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="168"/>
       <c r="G5" s="169" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="170"/>
       <c r="C6" s="171" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="172"/>
       <c r="E6" s="173"/>
@@ -11229,11 +11224,11 @@
     <row r="7" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="164"/>
       <c r="C7" s="165" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="175"/>
       <c r="E7" s="176" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="177"/>
       <c r="G7" s="178"/>
@@ -11242,38 +11237,38 @@
       <c r="B8" s="164"/>
       <c r="C8" s="179"/>
       <c r="D8" s="180" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="180" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="180" t="s">
+      <c r="F8" s="180" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="180" t="s">
+      <c r="G8" s="181" t="s">
         <v>59</v>
-      </c>
-      <c r="G8" s="181" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="164"/>
       <c r="C9" s="179"/>
       <c r="D9" s="182" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="182" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="182" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="182" t="s">
+      <c r="G9" s="182" t="s">
         <v>62</v>
-      </c>
-      <c r="G9" s="182" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="164"/>
       <c r="C10" s="169" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="183"/>
       <c r="E10" s="184"/>
@@ -11290,7 +11285,7 @@
     <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="164"/>
       <c r="C11" s="169" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="183"/>
       <c r="E11" s="184"/>
@@ -11307,7 +11302,7 @@
     <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="164"/>
       <c r="C12" s="169" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="183"/>
       <c r="E12" s="184"/>
@@ -11324,7 +11319,7 @@
     <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="164"/>
       <c r="C13" s="169" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="183"/>
       <c r="E13" s="184"/>
@@ -11341,7 +11336,7 @@
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="164"/>
       <c r="C14" s="169" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="183"/>
       <c r="E14" s="184"/>
@@ -11358,13 +11353,13 @@
     <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="164"/>
       <c r="C15" s="169" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="187" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="188" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="185"/>
       <c r="G15" s="186"/>
@@ -11379,7 +11374,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="170"/>
       <c r="C16" s="171" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="172"/>
       <c r="E16" s="173"/>
@@ -11390,13 +11385,13 @@
       <c r="B17" s="164"/>
       <c r="C17" s="179"/>
       <c r="D17" s="189" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="189" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="189" t="s">
-        <v>58</v>
-      </c>
       <c r="F17" s="190" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="191"/>
     </row>
@@ -11404,20 +11399,20 @@
       <c r="B18" s="164"/>
       <c r="C18" s="179"/>
       <c r="D18" s="182" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="182" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F18" s="192" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="191"/>
     </row>
     <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="164"/>
       <c r="C19" s="165" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="185"/>
       <c r="E19" s="184"/>
@@ -11427,7 +11422,7 @@
     <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="164"/>
       <c r="C20" s="165" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="185"/>
       <c r="E20" s="184"/>
@@ -11437,7 +11432,7 @@
     <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="164"/>
       <c r="C21" s="165" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="185"/>
       <c r="E21" s="184"/>
@@ -11447,7 +11442,7 @@
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="164"/>
       <c r="C22" s="165" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="185"/>
       <c r="E22" s="184"/>
@@ -11457,7 +11452,7 @@
     <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="164"/>
       <c r="C23" s="165" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="185"/>
       <c r="E23" s="184"/>
@@ -11467,7 +11462,7 @@
     <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="164"/>
       <c r="C24" s="165" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="185"/>
       <c r="E24" s="184"/>
@@ -11477,7 +11472,7 @@
     <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="164"/>
       <c r="C25" s="165" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="185"/>
       <c r="E25" s="184"/>
@@ -11487,7 +11482,7 @@
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="164"/>
       <c r="C26" s="165" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D26" s="185"/>
       <c r="E26" s="184"/>
@@ -11497,7 +11492,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="161"/>
       <c r="C27" s="162" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="163"/>
       <c r="E27" s="163"/>
@@ -11507,7 +11502,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="164"/>
       <c r="C28" s="169" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D28" s="194"/>
       <c r="E28" s="194"/>
@@ -11526,29 +11521,29 @@
       <c r="B30" s="164"/>
       <c r="C30" s="198"/>
       <c r="D30" s="199" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="180" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="180" t="s">
+      <c r="F30" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="F30" s="180" t="s">
+      <c r="G30" s="180" t="s">
         <v>84</v>
-      </c>
-      <c r="G30" s="180" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="164"/>
       <c r="C31" s="198"/>
       <c r="D31" s="200" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="189" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="189" t="s">
+      <c r="F31" s="189" t="s">
         <v>87</v>
-      </c>
-      <c r="F31" s="189" t="s">
-        <v>88</v>
       </c>
       <c r="G31" s="189"/>
     </row>
@@ -11556,22 +11551,22 @@
       <c r="B32" s="164"/>
       <c r="C32" s="198"/>
       <c r="D32" s="201" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="182" t="s">
         <v>89</v>
       </c>
-      <c r="E32" s="182" t="s">
+      <c r="F32" s="182" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="202" t="s">
         <v>90</v>
-      </c>
-      <c r="F32" s="182" t="s">
-        <v>33</v>
-      </c>
-      <c r="G32" s="202" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="164"/>
       <c r="C33" s="169" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="203"/>
       <c r="E33" s="204"/>
@@ -11581,35 +11576,35 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="164"/>
       <c r="C34" s="169" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="203"/>
       <c r="E34" s="204"/>
       <c r="F34" s="206" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34" s="207" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="195"/>
       <c r="C35" s="208" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" s="209"/>
       <c r="E35" s="210"/>
       <c r="F35" s="211" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G35" s="212" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="164"/>
       <c r="C36" s="213" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36" s="213"/>
       <c r="E36" s="214"/>
@@ -11619,7 +11614,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="161"/>
       <c r="C37" s="162" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D37" s="163"/>
       <c r="E37" s="163"/>
@@ -11629,7 +11624,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="164"/>
       <c r="C38" s="165" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D38" s="215"/>
       <c r="E38" s="215"/>
@@ -11648,52 +11643,52 @@
       <c r="B40" s="217"/>
       <c r="C40" s="218"/>
       <c r="D40" s="180" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="219" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="219" t="s">
+      <c r="F40" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="180" t="s">
+      <c r="G40" s="180" t="s">
         <v>99</v>
-      </c>
-      <c r="G40" s="180" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="164"/>
       <c r="C41" s="179"/>
       <c r="D41" s="189" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E41" s="220" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F41" s="189"/>
       <c r="G41" s="189" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="164"/>
       <c r="C42" s="179"/>
       <c r="D42" s="221" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" s="221" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F42" s="221" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G42" s="182" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="164"/>
       <c r="C43" s="165" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" s="222"/>
       <c r="E43" s="222"/>
@@ -11703,7 +11698,7 @@
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="164"/>
       <c r="C44" s="165" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D44" s="222"/>
       <c r="E44" s="222"/>
@@ -11713,7 +11708,7 @@
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="164"/>
       <c r="C45" s="223" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" s="224"/>
       <c r="E45" s="224"/>
@@ -11723,7 +11718,7 @@
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="164"/>
       <c r="C46" s="223" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D46" s="165"/>
       <c r="E46" s="165"/>
@@ -11743,10 +11738,10 @@
       <c r="B48" s="164"/>
       <c r="C48" s="179"/>
       <c r="D48" s="180" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" s="180" t="s">
         <v>107</v>
-      </c>
-      <c r="E48" s="180" t="s">
-        <v>108</v>
       </c>
       <c r="F48" s="228"/>
       <c r="G48" s="197"/>
@@ -11755,10 +11750,10 @@
       <c r="B49" s="164"/>
       <c r="C49" s="179"/>
       <c r="D49" s="182" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" s="182" t="s">
         <v>109</v>
-      </c>
-      <c r="E49" s="182" t="s">
-        <v>110</v>
       </c>
       <c r="F49" s="228"/>
       <c r="G49" s="197"/>
@@ -11766,7 +11761,7 @@
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="164"/>
       <c r="C50" s="165" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D50" s="204"/>
       <c r="E50" s="204"/>
@@ -11776,7 +11771,7 @@
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="164"/>
       <c r="C51" s="165" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D51" s="204"/>
       <c r="E51" s="204"/>
@@ -11786,7 +11781,7 @@
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="161"/>
       <c r="C52" s="162" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D52" s="163"/>
       <c r="E52" s="163"/>
@@ -11797,7 +11792,7 @@
       <c r="B53" s="164"/>
       <c r="C53" s="179"/>
       <c r="D53" s="229" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E53" s="200"/>
       <c r="F53" s="200"/>
@@ -11807,7 +11802,7 @@
       <c r="B54" s="164"/>
       <c r="C54" s="179"/>
       <c r="D54" s="230" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E54" s="230"/>
       <c r="F54" s="200"/>
@@ -11816,7 +11811,7 @@
     <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="164"/>
       <c r="C55" s="165" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" s="193"/>
       <c r="E55" s="231"/>
@@ -11826,7 +11821,7 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="161"/>
       <c r="C56" s="162" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56" s="163"/>
       <c r="E56" s="163"/>
@@ -11837,10 +11832,10 @@
       <c r="B57" s="164"/>
       <c r="C57" s="196"/>
       <c r="D57" s="232" t="s">
+        <v>115</v>
+      </c>
+      <c r="E57" s="233" t="s">
         <v>116</v>
-      </c>
-      <c r="E57" s="233" t="s">
-        <v>117</v>
       </c>
       <c r="F57" s="196"/>
       <c r="G57" s="197"/>
@@ -11849,10 +11844,10 @@
       <c r="B58" s="164"/>
       <c r="C58" s="179"/>
       <c r="D58" s="234" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E58" s="182" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F58" s="196"/>
       <c r="G58" s="197"/>
@@ -11860,7 +11855,7 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="164"/>
       <c r="C59" s="165" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D59" s="235"/>
       <c r="E59" s="236"/>
@@ -11870,7 +11865,7 @@
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="161"/>
       <c r="C60" s="162" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D60" s="163"/>
       <c r="E60" s="163"/>
@@ -11881,32 +11876,32 @@
       <c r="B61" s="164"/>
       <c r="C61" s="179"/>
       <c r="D61" s="189" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" s="189" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="189" t="s">
+      <c r="F61" s="228" t="s">
         <v>121</v>
       </c>
-      <c r="F61" s="228" t="s">
+      <c r="G61" s="189" t="s">
         <v>122</v>
-      </c>
-      <c r="G61" s="189" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="164"/>
       <c r="C62" s="179"/>
       <c r="D62" s="182" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E62" s="182" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F62" s="234" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G62" s="182" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12470,7 +12465,7 @@
     <row r="2" s="51" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="243"/>
       <c r="C2" s="244" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D2" s="245"/>
       <c r="E2" s="244"/>
@@ -12517,7 +12512,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="247"/>
       <c r="C3" s="248" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="249"/>
       <c r="E3" s="249"/>
@@ -12527,7 +12522,7 @@
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="164"/>
       <c r="C4" s="251" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="252"/>
       <c r="E4" s="252"/>
@@ -12553,7 +12548,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="164"/>
       <c r="C7" s="255" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="167"/>
       <c r="E7" s="256"/>
@@ -12563,7 +12558,7 @@
     <row r="8" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="164"/>
       <c r="C8" s="255" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8" s="167"/>
       <c r="E8" s="257"/>
@@ -12573,7 +12568,7 @@
     <row r="9" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="164"/>
       <c r="C9" s="229" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="258"/>
       <c r="E9" s="135"/>
@@ -12595,7 +12590,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="247"/>
       <c r="C11" s="248" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="249"/>
       <c r="E11" s="249"/>
@@ -12613,16 +12608,16 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="164"/>
       <c r="C13" s="257" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="189" t="s">
         <v>129</v>
       </c>
-      <c r="D13" s="189" t="s">
+      <c r="E13" s="189" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="189" t="s">
+      <c r="F13" s="190" t="s">
         <v>131</v>
-      </c>
-      <c r="F13" s="190" t="s">
-        <v>132</v>
       </c>
       <c r="G13" s="190"/>
     </row>
@@ -12630,13 +12625,13 @@
       <c r="B14" s="164"/>
       <c r="C14" s="179"/>
       <c r="D14" s="189" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" s="189" t="s">
         <v>133</v>
       </c>
-      <c r="E14" s="189" t="s">
+      <c r="F14" s="190" t="s">
         <v>134</v>
-      </c>
-      <c r="F14" s="190" t="s">
-        <v>135</v>
       </c>
       <c r="G14" s="190"/>
     </row>
@@ -12644,16 +12639,16 @@
       <c r="B15" s="195"/>
       <c r="C15" s="261"/>
       <c r="D15" s="182" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="182" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="234" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="192" t="s">
         <v>33</v>
-      </c>
-      <c r="F15" s="234" t="s">
-        <v>136</v>
-      </c>
-      <c r="G15" s="192" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12667,7 +12662,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="164"/>
       <c r="C17" s="262" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="236"/>
       <c r="E17" s="263"/>
@@ -12677,7 +12672,7 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="164"/>
       <c r="C18" s="262" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="236"/>
       <c r="E18" s="263"/>
@@ -12687,7 +12682,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="164"/>
       <c r="C19" s="264" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="236"/>
       <c r="E19" s="263"/>
@@ -12697,7 +12692,7 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="164"/>
       <c r="C20" s="264" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="236"/>
       <c r="E20" s="263"/>
@@ -12707,7 +12702,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="164"/>
       <c r="C21" s="265" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="236"/>
       <c r="E21" s="263"/>
@@ -12717,7 +12712,7 @@
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="164"/>
       <c r="C22" s="257" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D22" s="266"/>
       <c r="E22" s="267"/>
@@ -12735,7 +12730,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="247"/>
       <c r="C24" s="248" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D24" s="163"/>
       <c r="E24" s="249"/>
@@ -12755,10 +12750,10 @@
       <c r="C26" s="179"/>
       <c r="D26" s="198"/>
       <c r="E26" s="188" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="188" t="s">
         <v>31</v>
-      </c>
-      <c r="F26" s="188" t="s">
-        <v>32</v>
       </c>
       <c r="G26" s="197"/>
     </row>
@@ -12773,7 +12768,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="164"/>
       <c r="C28" s="270" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D28" s="270"/>
       <c r="E28" s="236"/>
@@ -12783,7 +12778,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="164"/>
       <c r="C29" s="270" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D29" s="270"/>
       <c r="E29" s="236"/>
@@ -12793,7 +12788,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="164"/>
       <c r="C30" s="272" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D30" s="272"/>
       <c r="E30" s="236"/>
@@ -12803,7 +12798,7 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="164"/>
       <c r="C31" s="272" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D31" s="272"/>
       <c r="E31" s="236"/>
@@ -12813,7 +12808,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="164"/>
       <c r="C32" s="272" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D32" s="272"/>
       <c r="E32" s="236"/>
@@ -12823,7 +12818,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="164"/>
       <c r="C33" s="272" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D33" s="272"/>
       <c r="E33" s="236"/>
@@ -12841,7 +12836,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="247"/>
       <c r="C35" s="248" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D35" s="249"/>
       <c r="E35" s="249"/>
@@ -12861,13 +12856,13 @@
       <c r="C37" s="179"/>
       <c r="D37" s="179"/>
       <c r="E37" s="189" t="s">
+        <v>145</v>
+      </c>
+      <c r="F37" s="189" t="s">
         <v>146</v>
       </c>
-      <c r="F37" s="189" t="s">
+      <c r="G37" s="189" t="s">
         <v>147</v>
-      </c>
-      <c r="G37" s="189" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12875,13 +12870,13 @@
       <c r="C38" s="179"/>
       <c r="D38" s="179"/>
       <c r="E38" s="188" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F38" s="188" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G38" s="188" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="6.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12895,7 +12890,7 @@
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="164"/>
       <c r="C40" s="165" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D40" s="165"/>
       <c r="E40" s="273"/>
@@ -12905,57 +12900,57 @@
     <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="164"/>
       <c r="C41" s="165" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D41" s="165"/>
       <c r="E41" s="236"/>
       <c r="F41" s="236"/>
       <c r="G41" s="189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="164"/>
       <c r="C42" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D42" s="165"/>
       <c r="E42" s="236"/>
       <c r="F42" s="236"/>
       <c r="G42" s="189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="164"/>
       <c r="C43" s="165" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D43" s="165"/>
       <c r="E43" s="236"/>
       <c r="F43" s="236"/>
       <c r="G43" s="189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="164"/>
       <c r="C44" s="165" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D44" s="165"/>
       <c r="E44" s="236"/>
       <c r="F44" s="189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G44" s="189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="164"/>
       <c r="C45" s="165" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D45" s="165"/>
       <c r="E45" s="236"/>
@@ -12965,21 +12960,21 @@
     <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="164"/>
       <c r="C46" s="165" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D46" s="165"/>
       <c r="E46" s="236"/>
       <c r="F46" s="189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G46" s="189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="20.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="164"/>
       <c r="C47" s="257" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D47" s="257"/>
       <c r="E47" s="206"/>
@@ -12989,7 +12984,7 @@
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="164"/>
       <c r="C48" s="223" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="257"/>
       <c r="E48" s="230"/>
@@ -13007,7 +13002,7 @@
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="247"/>
       <c r="C50" s="248" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D50" s="249"/>
       <c r="E50" s="249"/>
@@ -13027,10 +13022,10 @@
       <c r="C52" s="179"/>
       <c r="D52" s="179"/>
       <c r="E52" s="188" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="188" t="s">
         <v>31</v>
-      </c>
-      <c r="F52" s="188" t="s">
-        <v>32</v>
       </c>
       <c r="G52" s="188"/>
     </row>
@@ -13045,7 +13040,7 @@
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="164"/>
       <c r="C54" s="165" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D54" s="165"/>
       <c r="E54" s="236"/>
@@ -13055,7 +13050,7 @@
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="164"/>
       <c r="C55" s="165" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D55" s="165"/>
       <c r="E55" s="236"/>
@@ -13065,7 +13060,7 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="164"/>
       <c r="C56" s="165" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D56" s="165"/>
       <c r="E56" s="236"/>
@@ -13075,7 +13070,7 @@
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="164"/>
       <c r="C57" s="165" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D57" s="165"/>
       <c r="E57" s="236"/>
@@ -13093,7 +13088,7 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="164"/>
       <c r="C59" s="223" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D59" s="277"/>
       <c r="E59" s="278"/>
@@ -13103,7 +13098,7 @@
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="164"/>
       <c r="C60" s="223" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D60" s="277"/>
       <c r="E60" s="279"/>
@@ -13121,7 +13116,7 @@
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="247"/>
       <c r="C62" s="248" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D62" s="249"/>
       <c r="E62" s="249"/>
@@ -13141,10 +13136,10 @@
       <c r="C64" s="179"/>
       <c r="D64" s="179"/>
       <c r="E64" s="188" t="s">
+        <v>30</v>
+      </c>
+      <c r="F64" s="188" t="s">
         <v>31</v>
-      </c>
-      <c r="F64" s="188" t="s">
-        <v>32</v>
       </c>
       <c r="G64" s="189"/>
     </row>
@@ -13159,7 +13154,7 @@
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="164"/>
       <c r="C66" s="165" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D66" s="165"/>
       <c r="E66" s="236"/>
@@ -13169,7 +13164,7 @@
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="164"/>
       <c r="C67" s="165" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D67" s="165"/>
       <c r="E67" s="236"/>
@@ -13179,7 +13174,7 @@
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="164"/>
       <c r="C68" s="165" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D68" s="165"/>
       <c r="E68" s="236"/>
@@ -13189,7 +13184,7 @@
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="164"/>
       <c r="C69" s="165" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D69" s="165"/>
       <c r="E69" s="236"/>
@@ -13199,7 +13194,7 @@
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="164"/>
       <c r="C70" s="165" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D70" s="165"/>
       <c r="E70" s="236"/>
@@ -13217,7 +13212,7 @@
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="247"/>
       <c r="C72" s="248" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D72" s="249"/>
       <c r="E72" s="249"/>
@@ -13235,7 +13230,7 @@
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="164"/>
       <c r="C74" s="165" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D74" s="165"/>
       <c r="E74" s="281"/>
@@ -13769,7 +13764,7 @@
     <row r="2" s="283" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="284"/>
       <c r="C2" s="285" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D2" s="285"/>
       <c r="E2" s="286"/>
@@ -13829,7 +13824,7 @@
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="102"/>
       <c r="C3" s="288" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D3" s="288"/>
       <c r="E3" s="288"/>
@@ -13853,7 +13848,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="98"/>
       <c r="C5" s="99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D5" s="99"/>
       <c r="E5" s="100"/>
@@ -13912,17 +13907,17 @@
     <row r="10" s="283" customFormat="true" ht="21.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="291"/>
       <c r="C10" s="292" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="293"/>
       <c r="E10" s="294"/>
       <c r="F10" s="295"/>
       <c r="G10" s="296"/>
       <c r="H10" s="297" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="297" t="s">
         <v>31</v>
-      </c>
-      <c r="I10" s="297" t="s">
-        <v>32</v>
       </c>
       <c r="J10" s="297"/>
       <c r="AKP10" s="0"/>
@@ -13987,7 +13982,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="102"/>
       <c r="C12" s="105" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="105"/>
       <c r="E12" s="301"/>
@@ -14011,7 +14006,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="102"/>
       <c r="C14" s="105" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" s="105"/>
       <c r="E14" s="301"/>
@@ -14035,7 +14030,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="102"/>
       <c r="C16" s="305" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D16" s="105"/>
       <c r="E16" s="301"/>
@@ -14048,7 +14043,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="102"/>
       <c r="C17" s="305" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" s="105"/>
       <c r="E17" s="301"/>
@@ -14072,7 +14067,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="102"/>
       <c r="C19" s="105" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D19" s="105"/>
       <c r="E19" s="105"/>
@@ -14096,23 +14091,23 @@
     <row r="21" s="283" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="291"/>
       <c r="C21" s="292" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D21" s="292"/>
       <c r="E21" s="310" t="s">
+        <v>173</v>
+      </c>
+      <c r="F21" s="311" t="s">
         <v>174</v>
       </c>
-      <c r="F21" s="311" t="s">
+      <c r="G21" s="310" t="s">
         <v>175</v>
       </c>
-      <c r="G21" s="310" t="s">
-        <v>176</v>
-      </c>
       <c r="H21" s="311" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="311" t="s">
         <v>31</v>
-      </c>
-      <c r="I21" s="311" t="s">
-        <v>32</v>
       </c>
       <c r="J21" s="311"/>
       <c r="AKP21" s="0"/>
@@ -14177,12 +14172,12 @@
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="102"/>
       <c r="C23" s="105" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D23" s="105"/>
       <c r="E23" s="236"/>
       <c r="F23" s="319" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G23" s="320" t="n">
         <v>10</v>
@@ -14194,12 +14189,12 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="102"/>
       <c r="C24" s="105" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D24" s="105"/>
       <c r="E24" s="236"/>
       <c r="F24" s="319" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G24" s="320" t="n">
         <v>1300</v>
@@ -14211,12 +14206,12 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="102"/>
       <c r="C25" s="105" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" s="105"/>
       <c r="E25" s="236"/>
       <c r="F25" s="319" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G25" s="320" t="n">
         <v>1700</v>
@@ -14228,12 +14223,12 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="102"/>
       <c r="C26" s="105" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D26" s="105"/>
       <c r="E26" s="236"/>
       <c r="F26" s="319" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G26" s="320" t="n">
         <v>4.7</v>
@@ -14267,7 +14262,7 @@
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="102"/>
       <c r="C29" s="324" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D29" s="324"/>
       <c r="E29" s="236"/>
@@ -14335,7 +14330,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="102"/>
       <c r="C35" s="292" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D35" s="292"/>
       <c r="E35" s="301"/>
@@ -14353,10 +14348,10 @@
       <c r="F36" s="77"/>
       <c r="G36" s="301"/>
       <c r="H36" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="117" t="s">
         <v>31</v>
-      </c>
-      <c r="I36" s="117" t="s">
-        <v>32</v>
       </c>
       <c r="J36" s="117"/>
     </row>
@@ -14374,7 +14369,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="102"/>
       <c r="C38" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="341"/>
@@ -14398,7 +14393,7 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="102"/>
       <c r="C40" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="341"/>
@@ -14422,7 +14417,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="102"/>
       <c r="C42" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="341"/>
@@ -14446,7 +14441,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="102"/>
       <c r="C44" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="341"/>
@@ -14470,7 +14465,7 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="102"/>
       <c r="C46" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="4"/>
@@ -14494,7 +14489,7 @@
     <row r="48" customFormat="false" ht="19.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="96"/>
       <c r="C48" s="348" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D48" s="348"/>
       <c r="E48" s="348"/>
@@ -15062,7 +15057,7 @@
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" s="350" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="351" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="351"/>
       <c r="D2" s="351"/>
@@ -15101,7 +15096,7 @@
     </row>
     <row r="3" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="352" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3" s="352"/>
       <c r="D3" s="352"/>
@@ -15110,7 +15105,7 @@
     </row>
     <row r="4" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="353" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="99"/>
       <c r="D4" s="354"/>
@@ -15162,7 +15157,7 @@
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="357" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="357"/>
       <c r="D11" s="357"/>
@@ -15199,31 +15194,31 @@
     <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="360"/>
       <c r="C15" s="361" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="361" t="s">
         <v>194</v>
       </c>
-      <c r="D15" s="361" t="s">
+      <c r="E15" s="361" t="s">
         <v>195</v>
       </c>
-      <c r="E15" s="361" t="s">
+      <c r="F15" s="362" t="s">
         <v>196</v>
-      </c>
-      <c r="F15" s="362" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="363"/>
       <c r="C16" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15255,7 +15250,7 @@
     </row>
     <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="365" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C20" s="99"/>
       <c r="D20" s="354"/>
@@ -15308,7 +15303,7 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="357" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C27" s="357"/>
       <c r="D27" s="357"/>
@@ -15345,31 +15340,31 @@
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="367"/>
       <c r="C31" s="361" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D31" s="361" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" s="361" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="361" t="s">
-        <v>200</v>
-      </c>
       <c r="F31" s="362" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="367"/>
       <c r="C32" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F32" s="117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15401,7 +15396,7 @@
     </row>
     <row r="36" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="365" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C36" s="368"/>
       <c r="D36" s="13"/>
@@ -15452,7 +15447,7 @@
     </row>
     <row r="43" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="357" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C43" s="357"/>
       <c r="D43" s="357"/>
@@ -15489,31 +15484,31 @@
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="367"/>
       <c r="C47" s="361" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D47" s="361" t="s">
+        <v>198</v>
+      </c>
+      <c r="E47" s="361" t="s">
         <v>199</v>
       </c>
-      <c r="E47" s="361" t="s">
-        <v>200</v>
-      </c>
       <c r="F47" s="362" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="367"/>
       <c r="C48" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D48" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E48" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F48" s="117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15747,7 +15742,7 @@
     <row r="1" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="353" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C2" s="99"/>
       <c r="D2" s="354"/>
@@ -15807,7 +15802,7 @@
     </row>
     <row r="10" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="369" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="369"/>
       <c r="D10" s="369"/>
@@ -15844,31 +15839,31 @@
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="367"/>
       <c r="C14" s="361" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D14" s="361" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" s="361" t="s">
         <v>199</v>
       </c>
-      <c r="E14" s="361" t="s">
-        <v>200</v>
-      </c>
       <c r="F14" s="362" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="367"/>
       <c r="C15" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15900,7 +15895,7 @@
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="365" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C19" s="368"/>
       <c r="D19" s="13"/>
@@ -15958,7 +15953,7 @@
     </row>
     <row r="27" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="369" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C27" s="369"/>
       <c r="D27" s="369"/>
@@ -15995,31 +15990,31 @@
     <row r="31" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="367"/>
       <c r="C31" s="361" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D31" s="361" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" s="361" t="s">
         <v>199</v>
       </c>
-      <c r="E31" s="361" t="s">
-        <v>200</v>
-      </c>
       <c r="F31" s="362" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="367"/>
       <c r="C32" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" s="117" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F32" s="117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16051,7 +16046,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="371" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C36" s="371"/>
       <c r="D36" s="371"/>
@@ -16165,7 +16160,7 @@
     </row>
     <row r="52" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="353" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C52" s="99"/>
       <c r="D52" s="354"/>
@@ -16181,7 +16176,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="319" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C54" s="319"/>
       <c r="D54" s="319"/>
@@ -16358,7 +16353,7 @@
     <row r="1" customFormat="false" ht="7.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="374" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="374"/>
       <c r="D2" s="374"/>

</xml_diff>

<commit_message>
AE-375: replace footer text with energiatodistuksen tunnus
</commit_message>
<xml_diff>
--- a/etp-backend/src/main/resources/energiatodistus-template.xlsx
+++ b/etp-backend/src/main/resources/energiatodistus-template.xlsx
@@ -1588,7 +1588,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00000"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
-    <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
+    <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
     <numFmt numFmtId="168" formatCode="0%"/>
     <numFmt numFmtId="169" formatCode="[$-40B]0"/>
     <numFmt numFmtId="170" formatCode="[$-40B]0.00"/>
@@ -2380,7 +2380,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -6380,9 +6380,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>241560</xdr:colOff>
+      <xdr:colOff>241200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>255960</xdr:rowOff>
+      <xdr:rowOff>255600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6396,7 +6396,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4656960"/>
-          <a:ext cx="751680" cy="208440"/>
+          <a:ext cx="751320" cy="208080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6417,9 +6417,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>141480</xdr:colOff>
+      <xdr:colOff>141120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>255960</xdr:rowOff>
+      <xdr:rowOff>255600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6433,7 +6433,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="4971240"/>
-          <a:ext cx="1095120" cy="208440"/>
+          <a:ext cx="1094760" cy="208080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6454,9 +6454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>14760</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>255960</xdr:rowOff>
+      <xdr:rowOff>255600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6470,7 +6470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5285520"/>
-          <a:ext cx="1401840" cy="208440"/>
+          <a:ext cx="1401480" cy="208080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6491,9 +6491,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>338760</xdr:colOff>
+      <xdr:colOff>338400</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>255960</xdr:rowOff>
+      <xdr:rowOff>255600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6507,7 +6507,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5599800"/>
-          <a:ext cx="1725840" cy="208440"/>
+          <a:ext cx="1725480" cy="208080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6528,9 +6528,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>212040</xdr:colOff>
+      <xdr:colOff>211680</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>268920</xdr:rowOff>
+      <xdr:rowOff>268560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6544,7 +6544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="5909760"/>
-          <a:ext cx="2032920" cy="221400"/>
+          <a:ext cx="2032560" cy="221040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6565,9 +6565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>155160</xdr:colOff>
+      <xdr:colOff>154800</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>255960</xdr:rowOff>
+      <xdr:rowOff>255600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6581,7 +6581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6219720"/>
-          <a:ext cx="2369160" cy="208440"/>
+          <a:ext cx="2368800" cy="208080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6602,9 +6602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
+      <xdr:colOff>95040</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>255960</xdr:rowOff>
+      <xdr:rowOff>255600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6614,7 +6614,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1254240" y="6530400"/>
-          <a:ext cx="2682000" cy="207360"/>
+          <a:ext cx="2681640" cy="207000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6983,9 +6983,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>294840</xdr:colOff>
+      <xdr:colOff>294480</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>95040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6995,7 +6995,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="149400" y="78480"/>
-          <a:ext cx="6981120" cy="10550880"/>
+          <a:ext cx="6980760" cy="10550520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7128,9 +7128,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>141840</xdr:colOff>
+      <xdr:colOff>141480</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7140,7 +7140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="201240" y="10549800"/>
-          <a:ext cx="7016400" cy="250920"/>
+          <a:ext cx="7016040" cy="250560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7175,7 +7175,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>[Todistustunnus järjestelmästä], 2/8</a:t>
+            <a:t>Todistustunnus: [Todistustunnus järjestelmästä], 2/8</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -7199,9 +7199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1006560</xdr:colOff>
+      <xdr:colOff>1006200</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7211,7 +7211,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="396000" y="10928880"/>
-          <a:ext cx="7083720" cy="257400"/>
+          <a:ext cx="7083360" cy="257040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7246,7 +7246,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>[Todistustunnus järjestelmästä], 3/8</a:t>
+            <a:t>Todistustunnus: [Todistustunnus järjestelmästä], 3/8</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -7270,9 +7270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1010160</xdr:colOff>
+      <xdr:colOff>1009800</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7282,7 +7282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="290520" y="11094480"/>
-          <a:ext cx="7043400" cy="252360"/>
+          <a:ext cx="7043040" cy="252000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7317,7 +7317,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>[Todistustunnus järjestelmästä], 4/8</a:t>
+            <a:t>Todistustunnus: [Todistustunnus järjestelmästä], 4/8</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -7341,9 +7341,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>26640</xdr:colOff>
+      <xdr:colOff>26280</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7353,7 +7353,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="241920" y="9930960"/>
-          <a:ext cx="6882480" cy="251640"/>
+          <a:ext cx="6882120" cy="251280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7388,7 +7388,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>[Todistustunnus järjestelmästä], 5/8</a:t>
+            <a:t>Todistustunnus: [Todistustunnus järjestelmästä], 5/8</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -7412,9 +7412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>45360</xdr:colOff>
+      <xdr:colOff>45000</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7424,7 +7424,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="170640" y="10200240"/>
-          <a:ext cx="6978960" cy="352440"/>
+          <a:ext cx="6978600" cy="352080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7459,7 +7459,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>[Todistustunnus järjestelmästä], 6/8</a:t>
+            <a:t>Todistustunnus: [Todistustunnus järjestelmästä], 6/8</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -7483,9 +7483,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>54720</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7495,7 +7495,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="163440" y="10335960"/>
-          <a:ext cx="6987960" cy="363600"/>
+          <a:ext cx="6987600" cy="363240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7530,7 +7530,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>[Todistustunnus järjestelmästä], 7/8</a:t>
+            <a:t>Todistustunnus: [Todistustunnus järjestelmästä], 7/8</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -7554,9 +7554,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>74520</xdr:colOff>
+      <xdr:colOff>74160</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7566,7 +7566,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="90720" y="9993600"/>
-          <a:ext cx="7028280" cy="363600"/>
+          <a:ext cx="7027920" cy="363240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7601,7 +7601,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>[Todistustunnus järjestelmästä], 8/8</a:t>
+            <a:t>Todistustunnus: [Todistustunnus järjestelmästä], 8/8</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1050" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -7615,13 +7615,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -9157,13 +9157,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B1:AA65"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -11104,13 +11104,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B2:AMJ67"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -12441,13 +12441,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B2:AMJ76"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -13737,13 +13737,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B2:AMJ55"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
     </sheetView>
   </sheetViews>
@@ -15034,13 +15034,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
@@ -15719,13 +15719,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B1:G58"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -16330,13 +16330,13 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B1:I61"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>